<commit_message>
stochastic target penalty for local minima
</commit_message>
<xml_diff>
--- a/latest_version/output/june_update/results_spb.xlsx
+++ b/latest_version/output/june_update/results_spb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,20 +486,25 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>edp</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>debt_safeguard</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>deficit_resilience</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>binding_safeguard</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>binding</t>
         </is>
@@ -532,18 +537,21 @@
         <v>0.208</v>
       </c>
       <c r="H2" t="n">
-        <v>0.627</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
+        <v>0.62</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.781</v>
+      </c>
       <c r="J2" t="n">
         <v>-0.082</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="n">
         <v>-0.082</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.781</v>
       </c>
     </row>
@@ -574,18 +582,21 @@
         <v>0.416</v>
       </c>
       <c r="H3" t="n">
-        <v>0.428</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
+        <v>0.432</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.092</v>
+      </c>
       <c r="J3" t="n">
         <v>0.8139999999999999</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="n">
         <v>0.8139999999999999</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>1.092</v>
       </c>
     </row>
@@ -616,20 +627,23 @@
         <v>-3.373</v>
       </c>
       <c r="H4" t="n">
-        <v>-3.805</v>
-      </c>
-      <c r="I4" t="inlineStr"/>
+        <v>-3.795</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-3.029</v>
+      </c>
       <c r="J4" t="n">
         <v>-2.203</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>-2.203</v>
-      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
         <v>-2.203</v>
       </c>
+      <c r="O4" t="n">
+        <v>-2.203</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -658,19 +672,22 @@
         <v>-0.438</v>
       </c>
       <c r="H5" t="n">
-        <v>0.349</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
+        <v>0.362</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.362</v>
+      </c>
       <c r="J5" t="n">
         <v>-1.019</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="n">
         <v>-1.019</v>
       </c>
-      <c r="N5" t="n">
-        <v>0.349</v>
+      <c r="O5" t="n">
+        <v>0.362</v>
       </c>
     </row>
     <row r="6">
@@ -700,20 +717,23 @@
         <v>0.074</v>
       </c>
       <c r="H6" t="n">
-        <v>0.541</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
+        <v>0.54</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.636</v>
+      </c>
       <c r="J6" t="n">
         <v>1.777</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>1.777</v>
-      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
         <v>1.777</v>
       </c>
+      <c r="O6" t="n">
+        <v>1.777</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -742,20 +762,23 @@
         <v>-0.548</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.129</v>
-      </c>
-      <c r="I7" t="inlineStr"/>
+        <v>-1.121</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.203</v>
+      </c>
       <c r="J7" t="n">
         <v>0.331</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="n">
-        <v>0.331</v>
-      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
         <v>0.331</v>
       </c>
+      <c r="O7" t="n">
+        <v>0.331</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -784,19 +807,22 @@
         <v>-3.268</v>
       </c>
       <c r="H8" t="n">
-        <v>10</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
+        <v>-5.54</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-2.916</v>
+      </c>
       <c r="J8" t="n">
         <v>-1.193</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="n">
         <v>-1.193</v>
       </c>
-      <c r="N8" t="n">
-        <v>10</v>
+      <c r="O8" t="n">
+        <v>-1.193</v>
       </c>
     </row>
     <row r="9">
@@ -826,18 +852,23 @@
         <v>-3.407</v>
       </c>
       <c r="H9" t="n">
-        <v>-4.473</v>
-      </c>
-      <c r="I9" t="inlineStr"/>
+        <v>-4.474</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-3.052</v>
+      </c>
       <c r="J9" t="n">
         <v>-2.064</v>
       </c>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>-2.11</v>
+      </c>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="n">
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="n">
         <v>-2.064</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>-2.11</v>
       </c>
     </row>
@@ -870,20 +901,23 @@
       <c r="H10" t="n">
         <v>1.391</v>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>1.391</v>
+      </c>
       <c r="J10" t="n">
         <v>-0.384</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
         <v>2.794</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
-        <v>2.794</v>
-      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
         <v>2.794</v>
       </c>
+      <c r="O10" t="n">
+        <v>2.794</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -912,18 +946,21 @@
         <v>0.236</v>
       </c>
       <c r="H11" t="n">
-        <v>0.487</v>
-      </c>
-      <c r="I11" t="inlineStr"/>
+        <v>0.484</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.772</v>
+      </c>
       <c r="J11" t="n">
         <v>0.673</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="n">
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="n">
         <v>0.673</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>0.772</v>
       </c>
     </row>
@@ -956,16 +993,19 @@
       <c r="H12" t="n">
         <v>0.334</v>
       </c>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>0.417</v>
+      </c>
       <c r="J12" t="n">
         <v>-0.488</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="n">
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="n">
         <v>-0.488</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>0.417</v>
       </c>
     </row>
@@ -996,18 +1036,21 @@
         <v>1.167</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9379999999999999</v>
-      </c>
-      <c r="I13" t="inlineStr"/>
+        <v>0.883</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.869</v>
+      </c>
       <c r="J13" t="n">
         <v>1.745</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="n">
         <v>1.745</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>1.869</v>
       </c>
     </row>
@@ -1038,18 +1081,21 @@
         <v>2.616</v>
       </c>
       <c r="H14" t="n">
-        <v>2.804</v>
-      </c>
-      <c r="I14" t="inlineStr"/>
+        <v>2.81</v>
+      </c>
+      <c r="I14" t="n">
+        <v>3.049</v>
+      </c>
       <c r="J14" t="n">
         <v>2.316</v>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="n">
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="n">
         <v>2.316</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>3.049</v>
       </c>
     </row>
@@ -1080,20 +1126,23 @@
         <v>-2.346</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.411</v>
-      </c>
-      <c r="I15" t="inlineStr"/>
+        <v>-3.413</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-1.989</v>
+      </c>
       <c r="J15" t="n">
         <v>-0.626</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
-      <c r="M15" t="n">
-        <v>-0.626</v>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
         <v>-0.626</v>
       </c>
+      <c r="O15" t="n">
+        <v>-0.626</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1122,18 +1171,21 @@
         <v>2.542</v>
       </c>
       <c r="H16" t="n">
-        <v>2.459</v>
-      </c>
-      <c r="I16" t="inlineStr"/>
+        <v>2.462</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3.286</v>
+      </c>
       <c r="J16" t="n">
         <v>3.168</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
-      <c r="M16" t="n">
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="n">
         <v>3.168</v>
       </c>
-      <c r="N16" t="n">
+      <c r="O16" t="n">
         <v>3.286</v>
       </c>
     </row>
@@ -1164,18 +1216,21 @@
         <v>-1.293</v>
       </c>
       <c r="H17" t="n">
-        <v>-1.049</v>
-      </c>
-      <c r="I17" t="inlineStr"/>
+        <v>-1.056</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-0.952</v>
+      </c>
       <c r="J17" t="n">
         <v>-1.165</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
-      <c r="M17" t="n">
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="n">
         <v>-1.165</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>-0.952</v>
       </c>
     </row>
@@ -1206,20 +1261,23 @@
         <v>-1.114</v>
       </c>
       <c r="H18" t="n">
-        <v>-2</v>
-      </c>
-      <c r="I18" t="inlineStr"/>
+        <v>-1.997</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-0.765</v>
+      </c>
       <c r="J18" t="n">
         <v>0.015</v>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
-      <c r="M18" t="n">
-        <v>0.015</v>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
         <v>0.015</v>
       </c>
+      <c r="O18" t="n">
+        <v>0.015</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1248,20 +1306,23 @@
         <v>-3.422</v>
       </c>
       <c r="H19" t="n">
-        <v>-5.051</v>
-      </c>
-      <c r="I19" t="inlineStr"/>
+        <v>-5.058</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-3.058</v>
+      </c>
       <c r="J19" t="n">
         <v>-0.749</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
-      <c r="M19" t="n">
-        <v>-0.749</v>
-      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
         <v>-0.749</v>
       </c>
+      <c r="O19" t="n">
+        <v>-0.749</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1290,22 +1351,27 @@
         <v>-2.238</v>
       </c>
       <c r="H20" t="n">
-        <v>-1.913</v>
-      </c>
-      <c r="I20" t="inlineStr"/>
+        <v>-1.912</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-1.88</v>
+      </c>
       <c r="J20" t="n">
         <v>-1.253</v>
       </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="n">
-        <v>-0.996</v>
-      </c>
+      <c r="K20" t="n">
+        <v>-1.377</v>
+      </c>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
         <v>-0.996</v>
       </c>
       <c r="N20" t="n">
         <v>-0.996</v>
       </c>
+      <c r="O20" t="n">
+        <v>-0.996</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1334,20 +1400,23 @@
         <v>-0.908</v>
       </c>
       <c r="H21" t="n">
-        <v>-1.639</v>
-      </c>
-      <c r="I21" t="inlineStr"/>
+        <v>-1.636</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-0.5570000000000001</v>
+      </c>
       <c r="J21" t="n">
         <v>-0.28</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
-      <c r="M21" t="n">
-        <v>-0.28</v>
-      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
         <v>-0.28</v>
       </c>
+      <c r="O21" t="n">
+        <v>-0.28</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1376,19 +1445,22 @@
         <v>0.002</v>
       </c>
       <c r="H22" t="n">
-        <v>0.611</v>
-      </c>
-      <c r="I22" t="inlineStr"/>
+        <v>0.612</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.612</v>
+      </c>
       <c r="J22" t="n">
         <v>0.492</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
-      <c r="M22" t="n">
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="n">
         <v>0.492</v>
       </c>
-      <c r="N22" t="n">
-        <v>0.611</v>
+      <c r="O22" t="n">
+        <v>0.612</v>
       </c>
     </row>
     <row r="23">
@@ -1418,18 +1490,21 @@
         <v>2.028</v>
       </c>
       <c r="H23" t="n">
-        <v>1.965</v>
-      </c>
-      <c r="I23" t="inlineStr"/>
+        <v>1.984</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2.566</v>
+      </c>
       <c r="J23" t="n">
         <v>1.682</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
-      <c r="M23" t="n">
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="n">
         <v>1.682</v>
       </c>
-      <c r="N23" t="n">
+      <c r="O23" t="n">
         <v>2.566</v>
       </c>
     </row>
@@ -1460,20 +1535,23 @@
         <v>-0.643</v>
       </c>
       <c r="H24" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="I24" t="inlineStr"/>
+        <v>0.044</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.044</v>
+      </c>
       <c r="J24" t="n">
         <v>0.129</v>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
-      <c r="M24" t="n">
-        <v>0.129</v>
-      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
         <v>0.129</v>
       </c>
+      <c r="O24" t="n">
+        <v>0.129</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1502,18 +1580,21 @@
         <v>0.488</v>
       </c>
       <c r="H25" t="n">
-        <v>0.698</v>
-      </c>
-      <c r="I25" t="inlineStr"/>
+        <v>0.711</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.834</v>
+      </c>
       <c r="J25" t="n">
         <v>0.427</v>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="n">
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="n">
         <v>0.427</v>
       </c>
-      <c r="N25" t="n">
+      <c r="O25" t="n">
         <v>0.834</v>
       </c>
     </row>
@@ -1544,18 +1625,21 @@
         <v>0.162</v>
       </c>
       <c r="H26" t="n">
-        <v>0.336</v>
-      </c>
-      <c r="I26" t="inlineStr"/>
+        <v>0.33</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.515</v>
+      </c>
       <c r="J26" t="n">
         <v>0.372</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
-      <c r="M26" t="n">
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="n">
         <v>0.372</v>
       </c>
-      <c r="N26" t="n">
+      <c r="O26" t="n">
         <v>0.515</v>
       </c>
     </row>
@@ -1586,18 +1670,21 @@
         <v>2.095</v>
       </c>
       <c r="H27" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="I27" t="inlineStr"/>
+        <v>1.073</v>
+      </c>
+      <c r="I27" t="n">
+        <v>2.73</v>
+      </c>
       <c r="J27" t="n">
         <v>2.207</v>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
-      <c r="M27" t="n">
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="n">
         <v>2.207</v>
       </c>
-      <c r="N27" t="n">
+      <c r="O27" t="n">
         <v>2.73</v>
       </c>
     </row>
@@ -1628,18 +1715,23 @@
         <v>-2.635</v>
       </c>
       <c r="H28" t="n">
-        <v>-3.481</v>
-      </c>
-      <c r="I28" t="inlineStr"/>
+        <v>-3.475</v>
+      </c>
+      <c r="I28" t="n">
+        <v>-2.283</v>
+      </c>
       <c r="J28" t="n">
         <v>-1.014</v>
       </c>
-      <c r="K28" t="inlineStr"/>
+      <c r="K28" t="n">
+        <v>-1.196</v>
+      </c>
       <c r="L28" t="inlineStr"/>
-      <c r="M28" t="n">
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="n">
         <v>-1.014</v>
       </c>
-      <c r="N28" t="n">
+      <c r="O28" t="n">
         <v>-1.196</v>
       </c>
     </row>
@@ -1670,19 +1762,22 @@
         <v>-0.037</v>
       </c>
       <c r="H29" t="n">
-        <v>0.718</v>
-      </c>
-      <c r="I29" t="inlineStr"/>
+        <v>0.701</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.701</v>
+      </c>
       <c r="J29" t="n">
         <v>-0.239</v>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
-      <c r="M29" t="n">
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="n">
         <v>-0.239</v>
       </c>
-      <c r="N29" t="n">
-        <v>0.718</v>
+      <c r="O29" t="n">
+        <v>0.701</v>
       </c>
     </row>
     <row r="30">
@@ -1712,18 +1807,23 @@
         <v>0.451</v>
       </c>
       <c r="H30" t="n">
-        <v>0.653</v>
-      </c>
-      <c r="I30" t="inlineStr"/>
+        <v>0.661</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1.135</v>
+      </c>
       <c r="J30" t="n">
         <v>0.923</v>
       </c>
-      <c r="K30" t="inlineStr"/>
+      <c r="K30" t="n">
+        <v>1.13</v>
+      </c>
       <c r="L30" t="inlineStr"/>
-      <c r="M30" t="n">
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="n">
         <v>0.923</v>
       </c>
-      <c r="N30" t="n">
+      <c r="O30" t="n">
         <v>1.13</v>
       </c>
     </row>
@@ -1754,20 +1854,23 @@
         <v>-2.605</v>
       </c>
       <c r="H31" t="n">
-        <v>-2.644</v>
-      </c>
-      <c r="I31" t="inlineStr"/>
+        <v>-2.639</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-2.32</v>
+      </c>
       <c r="J31" t="n">
         <v>-1.792</v>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
-      <c r="M31" t="n">
-        <v>-1.792</v>
-      </c>
+      <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
         <v>-1.792</v>
       </c>
+      <c r="O31" t="n">
+        <v>-1.792</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1796,19 +1899,22 @@
         <v>-0.278</v>
       </c>
       <c r="H32" t="n">
-        <v>0.536</v>
-      </c>
-      <c r="I32" t="inlineStr"/>
+        <v>0.547</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.547</v>
+      </c>
       <c r="J32" t="n">
         <v>-0.9320000000000001</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
-      <c r="M32" t="n">
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="n">
         <v>-0.9320000000000001</v>
       </c>
-      <c r="N32" t="n">
-        <v>0.536</v>
+      <c r="O32" t="n">
+        <v>0.547</v>
       </c>
     </row>
     <row r="33">
@@ -1838,20 +1944,23 @@
         <v>-0.368</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.378</v>
-      </c>
-      <c r="I33" t="inlineStr"/>
+        <v>-0.364</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-0.083</v>
+      </c>
       <c r="J33" t="n">
         <v>0.374</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
-      <c r="M33" t="n">
-        <v>0.374</v>
-      </c>
+      <c r="M33" t="inlineStr"/>
       <c r="N33" t="n">
         <v>0.374</v>
       </c>
+      <c r="O33" t="n">
+        <v>0.374</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1880,20 +1989,23 @@
         <v>-0.336</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.841</v>
-      </c>
-      <c r="I34" t="inlineStr"/>
+        <v>-0.847</v>
+      </c>
+      <c r="I34" t="n">
+        <v>-0.052</v>
+      </c>
       <c r="J34" t="n">
         <v>0.617</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
-      <c r="M34" t="n">
-        <v>0.617</v>
-      </c>
+      <c r="M34" t="inlineStr"/>
       <c r="N34" t="n">
         <v>0.617</v>
       </c>
+      <c r="O34" t="n">
+        <v>0.617</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1922,19 +2034,22 @@
         <v>-3.441</v>
       </c>
       <c r="H35" t="n">
-        <v>10</v>
-      </c>
-      <c r="I35" t="inlineStr"/>
+        <v>-5.266</v>
+      </c>
+      <c r="I35" t="n">
+        <v>-3.147</v>
+      </c>
       <c r="J35" t="n">
         <v>-1.571</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
-      <c r="M35" t="n">
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="n">
         <v>-1.571</v>
       </c>
-      <c r="N35" t="n">
-        <v>10</v>
+      <c r="O35" t="n">
+        <v>-1.571</v>
       </c>
     </row>
     <row r="36">
@@ -1964,18 +2079,23 @@
         <v>-3.076</v>
       </c>
       <c r="H36" t="n">
-        <v>-3.753</v>
-      </c>
-      <c r="I36" t="inlineStr"/>
+        <v>-3.752</v>
+      </c>
+      <c r="I36" t="n">
+        <v>-2.778</v>
+      </c>
       <c r="J36" t="n">
         <v>-1.931</v>
       </c>
-      <c r="K36" t="inlineStr"/>
+      <c r="K36" t="n">
+        <v>-1.991</v>
+      </c>
       <c r="L36" t="inlineStr"/>
-      <c r="M36" t="n">
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="n">
         <v>-1.931</v>
       </c>
-      <c r="N36" t="n">
+      <c r="O36" t="n">
         <v>-1.991</v>
       </c>
     </row>
@@ -2006,22 +2126,25 @@
         <v>0.491</v>
       </c>
       <c r="H37" t="n">
-        <v>0.989</v>
-      </c>
-      <c r="I37" t="inlineStr"/>
+        <v>0.99</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.99</v>
+      </c>
       <c r="J37" t="n">
         <v>-0.615</v>
       </c>
-      <c r="K37" t="n">
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="n">
         <v>2.597</v>
       </c>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="n">
-        <v>2.597</v>
-      </c>
+      <c r="M37" t="inlineStr"/>
       <c r="N37" t="n">
         <v>2.597</v>
       </c>
+      <c r="O37" t="n">
+        <v>2.597</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2050,22 +2173,27 @@
         <v>0.383</v>
       </c>
       <c r="H38" t="n">
-        <v>0.587</v>
-      </c>
-      <c r="I38" t="inlineStr"/>
+        <v>0.585</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.795</v>
+      </c>
       <c r="J38" t="n">
         <v>0.753</v>
       </c>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="n">
-        <v>0.8139999999999999</v>
-      </c>
+      <c r="K38" t="n">
+        <v>0.788</v>
+      </c>
+      <c r="L38" t="inlineStr"/>
       <c r="M38" t="n">
         <v>0.8139999999999999</v>
       </c>
       <c r="N38" t="n">
         <v>0.8139999999999999</v>
       </c>
+      <c r="O38" t="n">
+        <v>0.8139999999999999</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2094,18 +2222,21 @@
         <v>-0.159</v>
       </c>
       <c r="H39" t="n">
-        <v>0.107</v>
-      </c>
-      <c r="I39" t="inlineStr"/>
+        <v>0.098</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.149</v>
+      </c>
       <c r="J39" t="n">
         <v>-0.7</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
-      <c r="M39" t="n">
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="n">
         <v>-0.7</v>
       </c>
-      <c r="N39" t="n">
+      <c r="O39" t="n">
         <v>0.149</v>
       </c>
     </row>
@@ -2136,18 +2267,21 @@
         <v>1.41</v>
       </c>
       <c r="H40" t="n">
-        <v>1.956</v>
-      </c>
-      <c r="I40" t="inlineStr"/>
+        <v>1.953</v>
+      </c>
+      <c r="I40" t="n">
+        <v>2.108</v>
+      </c>
       <c r="J40" t="n">
         <v>2.056</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
-      <c r="M40" t="n">
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="n">
         <v>2.056</v>
       </c>
-      <c r="N40" t="n">
+      <c r="O40" t="n">
         <v>2.108</v>
       </c>
     </row>
@@ -2178,19 +2312,24 @@
         <v>3.009</v>
       </c>
       <c r="H41" t="n">
-        <v>3.293</v>
-      </c>
-      <c r="I41" t="inlineStr"/>
+        <v>3.32</v>
+      </c>
+      <c r="I41" t="n">
+        <v>3.32</v>
+      </c>
       <c r="J41" t="n">
         <v>2.762</v>
       </c>
-      <c r="K41" t="inlineStr"/>
+      <c r="K41" t="n">
+        <v>3.31</v>
+      </c>
       <c r="L41" t="inlineStr"/>
-      <c r="M41" t="n">
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="n">
         <v>2.762</v>
       </c>
-      <c r="N41" t="n">
-        <v>3.3</v>
+      <c r="O41" t="n">
+        <v>3.31</v>
       </c>
     </row>
     <row r="42">
@@ -2220,20 +2359,23 @@
         <v>-2.34</v>
       </c>
       <c r="H42" t="n">
-        <v>-3.336</v>
-      </c>
-      <c r="I42" t="inlineStr"/>
+        <v>-3.339</v>
+      </c>
+      <c r="I42" t="n">
+        <v>-2.042</v>
+      </c>
       <c r="J42" t="n">
         <v>-0.597</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
-      <c r="M42" t="n">
-        <v>-0.597</v>
-      </c>
+      <c r="M42" t="inlineStr"/>
       <c r="N42" t="n">
         <v>-0.597</v>
       </c>
+      <c r="O42" t="n">
+        <v>-0.597</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2262,18 +2404,23 @@
         <v>2.742</v>
       </c>
       <c r="H43" t="n">
-        <v>2.764</v>
-      </c>
-      <c r="I43" t="inlineStr"/>
+        <v>2.771</v>
+      </c>
+      <c r="I43" t="n">
+        <v>2.997</v>
+      </c>
       <c r="J43" t="n">
         <v>3.124</v>
       </c>
-      <c r="K43" t="inlineStr"/>
+      <c r="K43" t="n">
+        <v>3.104</v>
+      </c>
       <c r="L43" t="inlineStr"/>
-      <c r="M43" t="n">
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="n">
         <v>3.124</v>
       </c>
-      <c r="N43" t="n">
+      <c r="O43" t="n">
         <v>3.104</v>
       </c>
     </row>
@@ -2304,19 +2451,22 @@
         <v>-1.055</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.6919999999999999</v>
-      </c>
-      <c r="I44" t="inlineStr"/>
+        <v>-0.6879999999999999</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-0.6879999999999999</v>
+      </c>
       <c r="J44" t="n">
         <v>-1.159</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
-      <c r="M44" t="n">
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="n">
         <v>-1.159</v>
       </c>
-      <c r="N44" t="n">
-        <v>-0.6919999999999999</v>
+      <c r="O44" t="n">
+        <v>-0.6879999999999999</v>
       </c>
     </row>
     <row r="45">
@@ -2346,20 +2496,23 @@
         <v>-1.064</v>
       </c>
       <c r="H45" t="n">
-        <v>-1.732</v>
-      </c>
-      <c r="I45" t="inlineStr"/>
+        <v>-1.73</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-0.773</v>
+      </c>
       <c r="J45" t="n">
         <v>-0.155</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
-      <c r="M45" t="n">
-        <v>-0.155</v>
-      </c>
+      <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
         <v>-0.155</v>
       </c>
+      <c r="O45" t="n">
+        <v>-0.155</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2388,20 +2541,23 @@
         <v>-3.345</v>
       </c>
       <c r="H46" t="n">
-        <v>-4.689</v>
-      </c>
-      <c r="I46" t="inlineStr"/>
+        <v>-4.674</v>
+      </c>
+      <c r="I46" t="n">
+        <v>-3.037</v>
+      </c>
       <c r="J46" t="n">
         <v>-0.851</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="n">
-        <v>-0.851</v>
-      </c>
+      <c r="M46" t="inlineStr"/>
       <c r="N46" t="n">
         <v>-0.851</v>
       </c>
+      <c r="O46" t="n">
+        <v>-0.851</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2430,18 +2586,23 @@
         <v>-1.643</v>
       </c>
       <c r="H47" t="n">
-        <v>-1.367</v>
-      </c>
-      <c r="I47" t="inlineStr"/>
+        <v>-1.366</v>
+      </c>
+      <c r="I47" t="n">
+        <v>-1.341</v>
+      </c>
       <c r="J47" t="n">
         <v>-1</v>
       </c>
-      <c r="K47" t="inlineStr"/>
+      <c r="K47" t="n">
+        <v>-1.05</v>
+      </c>
       <c r="L47" t="inlineStr"/>
-      <c r="M47" t="n">
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="n">
         <v>-1</v>
       </c>
-      <c r="N47" t="n">
+      <c r="O47" t="n">
         <v>-1.05</v>
       </c>
     </row>
@@ -2472,20 +2633,23 @@
         <v>-0.916</v>
       </c>
       <c r="H48" t="n">
-        <v>-1.388</v>
-      </c>
-      <c r="I48" t="inlineStr"/>
+        <v>-1.386</v>
+      </c>
+      <c r="I48" t="n">
+        <v>-0.623</v>
+      </c>
       <c r="J48" t="n">
         <v>-0.392</v>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="n">
-        <v>-0.392</v>
-      </c>
+      <c r="M48" t="inlineStr"/>
       <c r="N48" t="n">
         <v>-0.392</v>
       </c>
+      <c r="O48" t="n">
+        <v>-0.392</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2514,22 +2678,27 @@
         <v>0.386</v>
       </c>
       <c r="H49" t="n">
-        <v>0.831</v>
-      </c>
-      <c r="I49" t="inlineStr"/>
+        <v>0.8110000000000001</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.8110000000000001</v>
+      </c>
       <c r="J49" t="n">
         <v>0.533</v>
       </c>
-      <c r="K49" t="inlineStr"/>
-      <c r="L49" t="n">
-        <v>0.894</v>
-      </c>
+      <c r="K49" t="n">
+        <v>0.8070000000000001</v>
+      </c>
+      <c r="L49" t="inlineStr"/>
       <c r="M49" t="n">
         <v>0.894</v>
       </c>
       <c r="N49" t="n">
         <v>0.894</v>
       </c>
+      <c r="O49" t="n">
+        <v>0.894</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2558,18 +2727,21 @@
         <v>1.79</v>
       </c>
       <c r="H50" t="n">
-        <v>2.171</v>
-      </c>
-      <c r="I50" t="inlineStr"/>
+        <v>2.196</v>
+      </c>
+      <c r="I50" t="n">
+        <v>2.289</v>
+      </c>
       <c r="J50" t="n">
         <v>1.461</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
-      <c r="M50" t="n">
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="n">
         <v>1.461</v>
       </c>
-      <c r="N50" t="n">
+      <c r="O50" t="n">
         <v>2.289</v>
       </c>
     </row>
@@ -2600,19 +2772,22 @@
         <v>0.097</v>
       </c>
       <c r="H51" t="n">
-        <v>0.844</v>
-      </c>
-      <c r="I51" t="inlineStr"/>
+        <v>0.854</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.854</v>
+      </c>
       <c r="J51" t="n">
         <v>0.36</v>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
-      <c r="M51" t="n">
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="n">
         <v>0.36</v>
       </c>
-      <c r="N51" t="n">
-        <v>0.844</v>
+      <c r="O51" t="n">
+        <v>0.854</v>
       </c>
     </row>
     <row r="52">
@@ -2642,18 +2817,21 @@
         <v>0.855</v>
       </c>
       <c r="H52" t="n">
-        <v>0.912</v>
-      </c>
-      <c r="I52" t="inlineStr"/>
+        <v>0.905</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1.144</v>
+      </c>
       <c r="J52" t="n">
         <v>0.5649999999999999</v>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
-      <c r="M52" t="n">
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="n">
         <v>0.5649999999999999</v>
       </c>
-      <c r="N52" t="n">
+      <c r="O52" t="n">
         <v>1.144</v>
       </c>
     </row>
@@ -2684,18 +2862,21 @@
         <v>0.216</v>
       </c>
       <c r="H53" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="I53" t="inlineStr"/>
+        <v>0.343</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.51</v>
+      </c>
       <c r="J53" t="n">
         <v>0.43</v>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
-      <c r="M53" t="n">
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="n">
         <v>0.43</v>
       </c>
-      <c r="N53" t="n">
+      <c r="O53" t="n">
         <v>0.51</v>
       </c>
     </row>
@@ -2726,18 +2907,21 @@
         <v>2.147</v>
       </c>
       <c r="H54" t="n">
-        <v>1.663</v>
-      </c>
-      <c r="I54" t="inlineStr"/>
+        <v>1.661</v>
+      </c>
+      <c r="I54" t="n">
+        <v>2.777</v>
+      </c>
       <c r="J54" t="n">
         <v>2.274</v>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
-      <c r="M54" t="n">
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="n">
         <v>2.274</v>
       </c>
-      <c r="N54" t="n">
+      <c r="O54" t="n">
         <v>2.777</v>
       </c>
     </row>
@@ -2768,18 +2952,23 @@
         <v>-2.733</v>
       </c>
       <c r="H55" t="n">
-        <v>-3.358</v>
-      </c>
-      <c r="I55" t="inlineStr"/>
+        <v>-3.36</v>
+      </c>
+      <c r="I55" t="n">
+        <v>-2.435</v>
+      </c>
       <c r="J55" t="n">
         <v>-1.6</v>
       </c>
-      <c r="K55" t="inlineStr"/>
+      <c r="K55" t="n">
+        <v>-1.828</v>
+      </c>
       <c r="L55" t="inlineStr"/>
-      <c r="M55" t="n">
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="n">
         <v>-1.6</v>
       </c>
-      <c r="N55" t="n">
+      <c r="O55" t="n">
         <v>-1.828</v>
       </c>
     </row>

</xml_diff>

<commit_message>
inst debt bug fix and clean up
</commit_message>
<xml_diff>
--- a/latest_version/output/june_update/results_spb.xlsx
+++ b/latest_version/output/june_update/results_spb.xlsx
@@ -525,34 +525,34 @@
         <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>0.185</v>
+        <v>0.188</v>
       </c>
       <c r="E2" t="n">
-        <v>0.781</v>
+        <v>0.784</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>0.208</v>
+        <v>0.21</v>
       </c>
       <c r="H2" t="n">
-        <v>0.629</v>
+        <v>0.622</v>
       </c>
       <c r="I2" t="n">
-        <v>0.781</v>
+        <v>0.784</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.082</v>
+        <v>-0.079</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
-        <v>-0.082</v>
+        <v>-0.079</v>
       </c>
       <c r="O2" t="n">
-        <v>0.781</v>
+        <v>0.784</v>
       </c>
     </row>
     <row r="3">
@@ -570,34 +570,34 @@
         <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>0.353</v>
+        <v>0.355</v>
       </c>
       <c r="E3" t="n">
-        <v>1.092</v>
+        <v>1.094</v>
       </c>
       <c r="F3" t="n">
-        <v>0.855</v>
+        <v>0.857</v>
       </c>
       <c r="G3" t="n">
-        <v>0.416</v>
+        <v>0.418</v>
       </c>
       <c r="H3" t="n">
-        <v>0.432</v>
+        <v>0.444</v>
       </c>
       <c r="I3" t="n">
-        <v>1.092</v>
+        <v>1.094</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8139999999999999</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
-        <v>0.8139999999999999</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="O3" t="n">
-        <v>1.092</v>
+        <v>1.094</v>
       </c>
     </row>
     <row r="4">
@@ -615,34 +615,34 @@
         <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.405</v>
+        <v>-3.413</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.125</v>
+        <v>-3.133</v>
       </c>
       <c r="F4" t="n">
-        <v>-3.029</v>
+        <v>-3.037</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.373</v>
+        <v>-3.381</v>
       </c>
       <c r="H4" t="n">
         <v>-3.785</v>
       </c>
       <c r="I4" t="n">
-        <v>-3.029</v>
+        <v>-3.037</v>
       </c>
       <c r="J4" t="n">
-        <v>-2.203</v>
+        <v>-2.211</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
-        <v>-2.203</v>
+        <v>-2.211</v>
       </c>
       <c r="O4" t="n">
-        <v>-2.203</v>
+        <v>-2.211</v>
       </c>
     </row>
     <row r="5">
@@ -660,34 +660,34 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.476</v>
+        <v>-0.479</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.108</v>
+        <v>-0.111</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.101</v>
+        <v>-0.104</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.438</v>
+        <v>-0.441</v>
       </c>
       <c r="H5" t="n">
-        <v>0.346</v>
+        <v>0.349</v>
       </c>
       <c r="I5" t="n">
-        <v>0.346</v>
+        <v>0.349</v>
       </c>
       <c r="J5" t="n">
-        <v>-1.019</v>
+        <v>-1.025</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
-        <v>-1.019</v>
+        <v>-1.025</v>
       </c>
       <c r="O5" t="n">
-        <v>0.346</v>
+        <v>0.349</v>
       </c>
     </row>
     <row r="6">
@@ -705,34 +705,34 @@
         <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.021</v>
+        <v>-0.114</v>
       </c>
       <c r="E6" t="n">
-        <v>0.328</v>
+        <v>0.232</v>
       </c>
       <c r="F6" t="n">
-        <v>0.354</v>
+        <v>0.268</v>
       </c>
       <c r="G6" t="n">
-        <v>0.02</v>
+        <v>-0.083</v>
       </c>
       <c r="H6" t="n">
-        <v>0.247</v>
+        <v>0.136</v>
       </c>
       <c r="I6" t="n">
-        <v>0.354</v>
+        <v>0.268</v>
       </c>
       <c r="J6" t="n">
-        <v>0.701</v>
+        <v>0.605</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
-        <v>0.701</v>
+        <v>0.605</v>
       </c>
       <c r="O6" t="n">
-        <v>0.701</v>
+        <v>0.605</v>
       </c>
     </row>
     <row r="7">
@@ -750,34 +750,34 @@
         <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.575</v>
+        <v>-0.57</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.266</v>
+        <v>-0.261</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.203</v>
+        <v>-0.198</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.548</v>
+        <v>-0.544</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.115</v>
+        <v>-1.097</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.203</v>
+        <v>-0.198</v>
       </c>
       <c r="J7" t="n">
-        <v>0.331</v>
+        <v>0.334</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
-        <v>0.331</v>
+        <v>0.334</v>
       </c>
       <c r="O7" t="n">
-        <v>0.331</v>
+        <v>0.334</v>
       </c>
     </row>
     <row r="8">
@@ -795,34 +795,34 @@
         <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.291</v>
+        <v>-3.248</v>
       </c>
       <c r="E8" t="n">
-        <v>-3.011</v>
+        <v>-2.967</v>
       </c>
       <c r="F8" t="n">
-        <v>-2.916</v>
+        <v>-2.872</v>
       </c>
       <c r="G8" t="n">
-        <v>-3.268</v>
+        <v>-3.225</v>
       </c>
       <c r="H8" t="n">
-        <v>-5.54</v>
+        <v>-5.511</v>
       </c>
       <c r="I8" t="n">
-        <v>-2.916</v>
+        <v>-2.872</v>
       </c>
       <c r="J8" t="n">
-        <v>-1.193</v>
+        <v>-1.152</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
-        <v>-1.193</v>
+        <v>-1.152</v>
       </c>
       <c r="O8" t="n">
-        <v>-1.193</v>
+        <v>-1.152</v>
       </c>
     </row>
     <row r="9">
@@ -840,36 +840,36 @@
         <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>-3.425</v>
+        <v>-3.426</v>
       </c>
       <c r="E9" t="n">
         <v>-3.188</v>
       </c>
       <c r="F9" t="n">
-        <v>-3.052</v>
+        <v>-3.053</v>
       </c>
       <c r="G9" t="n">
-        <v>-3.407</v>
+        <v>-3.408</v>
       </c>
       <c r="H9" t="n">
-        <v>-4.479</v>
+        <v>-4.476</v>
       </c>
       <c r="I9" t="n">
-        <v>-3.052</v>
+        <v>-3.053</v>
       </c>
       <c r="J9" t="n">
-        <v>-2.064</v>
+        <v>-2.065</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
-        <v>-2.064</v>
+        <v>-2.065</v>
       </c>
       <c r="N9" t="n">
-        <v>-2.064</v>
+        <v>-2.065</v>
       </c>
       <c r="O9" t="n">
-        <v>-2.064</v>
+        <v>-2.065</v>
       </c>
     </row>
     <row r="10">
@@ -887,36 +887,36 @@
         <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>0.664</v>
+        <v>0.667</v>
       </c>
       <c r="E10" t="n">
-        <v>1.139</v>
+        <v>1.143</v>
       </c>
       <c r="F10" t="n">
-        <v>1.192</v>
+        <v>1.195</v>
       </c>
       <c r="G10" t="n">
-        <v>0.797</v>
+        <v>0.8</v>
       </c>
       <c r="H10" t="n">
-        <v>1.381</v>
+        <v>1.393</v>
       </c>
       <c r="I10" t="n">
-        <v>1.381</v>
+        <v>1.393</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.384</v>
+        <v>-0.381</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
-        <v>4.31</v>
+        <v>4.314</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>4.31</v>
+        <v>4.314</v>
       </c>
       <c r="O10" t="n">
-        <v>4.31</v>
+        <v>4.314</v>
       </c>
     </row>
     <row r="11">
@@ -934,34 +934,34 @@
         <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.095</v>
+        <v>-0.08799999999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>0.772</v>
+        <v>0.778</v>
       </c>
       <c r="F11" t="n">
-        <v>0.495</v>
+        <v>0.504</v>
       </c>
       <c r="G11" t="n">
-        <v>0.236</v>
+        <v>0.244</v>
       </c>
       <c r="H11" t="n">
-        <v>0.482</v>
+        <v>0.486</v>
       </c>
       <c r="I11" t="n">
-        <v>0.772</v>
+        <v>0.778</v>
       </c>
       <c r="J11" t="n">
-        <v>0.673</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
-        <v>0.673</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="O11" t="n">
-        <v>0.772</v>
+        <v>0.778</v>
       </c>
     </row>
     <row r="12">
@@ -979,34 +979,34 @@
         <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>0.034</v>
+        <v>0.038</v>
       </c>
       <c r="E12" t="n">
-        <v>0.417</v>
+        <v>0.42</v>
       </c>
       <c r="F12" t="n">
-        <v>0.409</v>
+        <v>0.413</v>
       </c>
       <c r="G12" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.076</v>
       </c>
       <c r="H12" t="n">
-        <v>0.334</v>
+        <v>0.342</v>
       </c>
       <c r="I12" t="n">
-        <v>0.417</v>
+        <v>0.42</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.488</v>
+        <v>-0.487</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
-        <v>-0.488</v>
+        <v>-0.487</v>
       </c>
       <c r="O12" t="n">
-        <v>0.417</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="13">
@@ -1024,34 +1024,34 @@
         <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>1.068</v>
+        <v>0.959</v>
       </c>
       <c r="E13" t="n">
-        <v>1.869</v>
+        <v>1.735</v>
       </c>
       <c r="F13" t="n">
-        <v>1.557</v>
+        <v>1.447</v>
       </c>
       <c r="G13" t="n">
-        <v>1.167</v>
+        <v>1.051</v>
       </c>
       <c r="H13" t="n">
-        <v>0.897</v>
+        <v>0.852</v>
       </c>
       <c r="I13" t="n">
-        <v>1.869</v>
+        <v>1.735</v>
       </c>
       <c r="J13" t="n">
-        <v>1.745</v>
+        <v>1.633</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
-        <v>1.745</v>
+        <v>1.633</v>
       </c>
       <c r="O13" t="n">
-        <v>1.869</v>
+        <v>1.735</v>
       </c>
     </row>
     <row r="14">
@@ -1069,34 +1069,34 @@
         <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>2.592</v>
+        <v>2.607</v>
       </c>
       <c r="E14" t="n">
-        <v>3.049</v>
+        <v>3.064</v>
       </c>
       <c r="F14" t="n">
-        <v>3.047</v>
+        <v>3.065</v>
       </c>
       <c r="G14" t="n">
-        <v>2.616</v>
+        <v>2.631</v>
       </c>
       <c r="H14" t="n">
-        <v>2.816</v>
+        <v>2.835</v>
       </c>
       <c r="I14" t="n">
-        <v>3.049</v>
+        <v>3.065</v>
       </c>
       <c r="J14" t="n">
-        <v>2.316</v>
+        <v>2.332</v>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
-        <v>2.316</v>
+        <v>2.332</v>
       </c>
       <c r="O14" t="n">
-        <v>3.049</v>
+        <v>3.065</v>
       </c>
     </row>
     <row r="15">
@@ -1114,34 +1114,34 @@
         <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.37</v>
+        <v>-2.377</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.079</v>
+        <v>-2.09</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.989</v>
+        <v>-1.996</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.346</v>
+        <v>-2.354</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.413</v>
+        <v>-3.412</v>
       </c>
       <c r="I15" t="n">
-        <v>-1.989</v>
+        <v>-1.996</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.626</v>
+        <v>-0.636</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>-0.626</v>
+        <v>-0.636</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.626</v>
+        <v>-0.636</v>
       </c>
     </row>
     <row r="16">
@@ -1159,34 +1159,34 @@
         <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>2.224</v>
+        <v>2.226</v>
       </c>
       <c r="E16" t="n">
-        <v>3.286</v>
+        <v>3.288</v>
       </c>
       <c r="F16" t="n">
-        <v>2.703</v>
+        <v>2.705</v>
       </c>
       <c r="G16" t="n">
-        <v>2.542</v>
+        <v>2.544</v>
       </c>
       <c r="H16" t="n">
-        <v>2.471</v>
+        <v>2.478</v>
       </c>
       <c r="I16" t="n">
-        <v>3.286</v>
+        <v>3.288</v>
       </c>
       <c r="J16" t="n">
-        <v>3.168</v>
+        <v>3.17</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
-        <v>3.168</v>
+        <v>3.17</v>
       </c>
       <c r="O16" t="n">
-        <v>3.286</v>
+        <v>3.288</v>
       </c>
     </row>
     <row r="17">
@@ -1210,16 +1210,16 @@
         <v>-0.998</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.952</v>
+        <v>-0.951</v>
       </c>
       <c r="G17" t="n">
         <v>-1.293</v>
       </c>
       <c r="H17" t="n">
-        <v>-1.061</v>
+        <v>-1.067</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.952</v>
+        <v>-0.951</v>
       </c>
       <c r="J17" t="n">
         <v>-1.165</v>
@@ -1231,7 +1231,7 @@
         <v>-1.165</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.952</v>
+        <v>-0.951</v>
       </c>
     </row>
     <row r="18">
@@ -1249,34 +1249,34 @@
         <v>4</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.142</v>
+        <v>-1.151</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.841</v>
+        <v>-0.849</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.765</v>
+        <v>-0.773</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.114</v>
+        <v>-1.122</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.996</v>
+        <v>-2.001</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.765</v>
+        <v>-0.773</v>
       </c>
       <c r="J18" t="n">
-        <v>0.015</v>
+        <v>0.005</v>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
-        <v>0.015</v>
+        <v>0.005</v>
       </c>
       <c r="O18" t="n">
-        <v>0.015</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="19">
@@ -1294,34 +1294,34 @@
         <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>-3.438</v>
+        <v>-3.441</v>
       </c>
       <c r="E19" t="n">
-        <v>-3.207</v>
+        <v>-3.21</v>
       </c>
       <c r="F19" t="n">
-        <v>-3.058</v>
+        <v>-3.06</v>
       </c>
       <c r="G19" t="n">
-        <v>-3.422</v>
+        <v>-3.424</v>
       </c>
       <c r="H19" t="n">
-        <v>-5.055</v>
+        <v>-5.064</v>
       </c>
       <c r="I19" t="n">
-        <v>-3.058</v>
+        <v>-3.06</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.75</v>
+        <v>-0.751</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
-        <v>-0.75</v>
+        <v>-0.751</v>
       </c>
       <c r="O19" t="n">
-        <v>-0.75</v>
+        <v>-0.751</v>
       </c>
     </row>
     <row r="20">
@@ -1339,38 +1339,38 @@
         <v>4</v>
       </c>
       <c r="D20" t="n">
-        <v>-2.267</v>
+        <v>-2.27</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.955</v>
+        <v>-1.958</v>
       </c>
       <c r="F20" t="n">
-        <v>-1.88</v>
+        <v>-1.883</v>
       </c>
       <c r="G20" t="n">
-        <v>-2.238</v>
+        <v>-2.241</v>
       </c>
       <c r="H20" t="n">
-        <v>-1.908</v>
+        <v>-1.907</v>
       </c>
       <c r="I20" t="n">
-        <v>-1.88</v>
+        <v>-1.883</v>
       </c>
       <c r="J20" t="n">
-        <v>-1.253</v>
+        <v>-1.252</v>
       </c>
       <c r="K20" t="n">
         <v>-1.377</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>-0.996</v>
+        <v>-0.997</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.996</v>
+        <v>-0.997</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.996</v>
+        <v>-0.997</v>
       </c>
     </row>
     <row r="21">
@@ -1388,34 +1388,34 @@
         <v>4</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.931</v>
+        <v>-0.928</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.636</v>
+        <v>-0.633</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.5570000000000001</v>
+        <v>-0.554</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.908</v>
+        <v>-0.905</v>
       </c>
       <c r="H21" t="n">
-        <v>-1.64</v>
+        <v>-1.633</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.5570000000000001</v>
+        <v>-0.554</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.28</v>
+        <v>-0.278</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
-        <v>-0.28</v>
+        <v>-0.278</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.28</v>
+        <v>-0.278</v>
       </c>
     </row>
     <row r="22">
@@ -1433,34 +1433,34 @@
         <v>4</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.039</v>
+        <v>-0.032</v>
       </c>
       <c r="E22" t="n">
-        <v>0.326</v>
+        <v>0.333</v>
       </c>
       <c r="F22" t="n">
-        <v>0.332</v>
+        <v>0.339</v>
       </c>
       <c r="G22" t="n">
-        <v>0.002</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="H22" t="n">
-        <v>0.609</v>
+        <v>0.617</v>
       </c>
       <c r="I22" t="n">
-        <v>0.609</v>
+        <v>0.617</v>
       </c>
       <c r="J22" t="n">
-        <v>0.492</v>
+        <v>0.502</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
-        <v>0.492</v>
+        <v>0.502</v>
       </c>
       <c r="O22" t="n">
-        <v>0.609</v>
+        <v>0.617</v>
       </c>
     </row>
     <row r="23">
@@ -1478,34 +1478,34 @@
         <v>4</v>
       </c>
       <c r="D23" t="n">
-        <v>2.013</v>
+        <v>1.967</v>
       </c>
       <c r="E23" t="n">
-        <v>2.566</v>
+        <v>2.507</v>
       </c>
       <c r="F23" t="n">
+        <v>2.461</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.983</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.966</v>
+      </c>
+      <c r="I23" t="n">
         <v>2.507</v>
       </c>
-      <c r="G23" t="n">
-        <v>2.028</v>
-      </c>
-      <c r="H23" t="n">
-        <v>1.98</v>
-      </c>
-      <c r="I23" t="n">
-        <v>2.566</v>
-      </c>
       <c r="J23" t="n">
-        <v>1.682</v>
+        <v>1.638</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="n">
-        <v>1.682</v>
+        <v>1.638</v>
       </c>
       <c r="O23" t="n">
-        <v>2.566</v>
+        <v>2.507</v>
       </c>
     </row>
     <row r="24">
@@ -1535,10 +1535,10 @@
         <v>-0.643</v>
       </c>
       <c r="H24" t="n">
-        <v>0.059</v>
+        <v>0.033</v>
       </c>
       <c r="I24" t="n">
-        <v>0.059</v>
+        <v>0.033</v>
       </c>
       <c r="J24" t="n">
         <v>0.129</v>
@@ -1568,34 +1568,34 @@
         <v>4</v>
       </c>
       <c r="D25" t="n">
-        <v>0.458</v>
+        <v>0.462</v>
       </c>
       <c r="E25" t="n">
-        <v>0.778</v>
+        <v>0.782</v>
       </c>
       <c r="F25" t="n">
-        <v>0.834</v>
+        <v>0.838</v>
       </c>
       <c r="G25" t="n">
-        <v>0.488</v>
+        <v>0.492</v>
       </c>
       <c r="H25" t="n">
-        <v>0.703</v>
+        <v>0.699</v>
       </c>
       <c r="I25" t="n">
-        <v>0.834</v>
+        <v>0.838</v>
       </c>
       <c r="J25" t="n">
-        <v>0.427</v>
+        <v>0.43</v>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
-        <v>0.427</v>
+        <v>0.43</v>
       </c>
       <c r="O25" t="n">
-        <v>0.834</v>
+        <v>0.838</v>
       </c>
     </row>
     <row r="26">
@@ -1613,22 +1613,22 @@
         <v>4</v>
       </c>
       <c r="D26" t="n">
-        <v>0.135</v>
+        <v>0.136</v>
       </c>
       <c r="E26" t="n">
-        <v>0.46</v>
+        <v>0.461</v>
       </c>
       <c r="F26" t="n">
-        <v>0.515</v>
+        <v>0.516</v>
       </c>
       <c r="G26" t="n">
-        <v>0.162</v>
+        <v>0.163</v>
       </c>
       <c r="H26" t="n">
-        <v>0.321</v>
+        <v>0.334</v>
       </c>
       <c r="I26" t="n">
-        <v>0.515</v>
+        <v>0.516</v>
       </c>
       <c r="J26" t="n">
         <v>0.372</v>
@@ -1640,7 +1640,7 @@
         <v>0.372</v>
       </c>
       <c r="O26" t="n">
-        <v>0.515</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="27">
@@ -1670,7 +1670,7 @@
         <v>2.095</v>
       </c>
       <c r="H27" t="n">
-        <v>1.075</v>
+        <v>1.088</v>
       </c>
       <c r="I27" t="n">
         <v>2.73</v>
@@ -1703,34 +1703,34 @@
         <v>4</v>
       </c>
       <c r="D28" t="n">
-        <v>-2.687</v>
+        <v>-3.315</v>
       </c>
       <c r="E28" t="n">
-        <v>-2.389</v>
+        <v>-3.041</v>
       </c>
       <c r="F28" t="n">
-        <v>-2.317</v>
+        <v>-2.937</v>
       </c>
       <c r="G28" t="n">
-        <v>-2.667</v>
+        <v>-3.308</v>
       </c>
       <c r="H28" t="n">
-        <v>-3.52</v>
+        <v>-4.643</v>
       </c>
       <c r="I28" t="n">
-        <v>-2.317</v>
+        <v>-2.937</v>
       </c>
       <c r="J28" t="n">
-        <v>-1.076</v>
+        <v>-2.094</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="n">
-        <v>-1.076</v>
+        <v>-2.094</v>
       </c>
       <c r="O28" t="n">
-        <v>-1.076</v>
+        <v>-2.094</v>
       </c>
     </row>
     <row r="29">
@@ -1748,34 +1748,34 @@
         <v>7</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.06</v>
+        <v>-0.059</v>
       </c>
       <c r="E29" t="n">
-        <v>0.55</v>
+        <v>0.551</v>
       </c>
       <c r="F29" t="n">
-        <v>0.449</v>
+        <v>0.45</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.037</v>
+        <v>-0.036</v>
       </c>
       <c r="H29" t="n">
-        <v>0.713</v>
+        <v>0.709</v>
       </c>
       <c r="I29" t="n">
-        <v>0.713</v>
+        <v>0.709</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.239</v>
+        <v>-0.237</v>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="n">
-        <v>-0.239</v>
+        <v>-0.237</v>
       </c>
       <c r="O29" t="n">
-        <v>0.713</v>
+        <v>0.709</v>
       </c>
     </row>
     <row r="30">
@@ -1793,36 +1793,36 @@
         <v>7</v>
       </c>
       <c r="D30" t="n">
-        <v>0.39</v>
+        <v>0.392</v>
       </c>
       <c r="E30" t="n">
-        <v>1.135</v>
+        <v>1.137</v>
       </c>
       <c r="F30" t="n">
-        <v>0.893</v>
+        <v>0.895</v>
       </c>
       <c r="G30" t="n">
-        <v>0.451</v>
+        <v>0.453</v>
       </c>
       <c r="H30" t="n">
-        <v>0.657</v>
+        <v>0.646</v>
       </c>
       <c r="I30" t="n">
-        <v>1.135</v>
+        <v>1.137</v>
       </c>
       <c r="J30" t="n">
-        <v>0.923</v>
+        <v>0.926</v>
       </c>
       <c r="K30" t="n">
-        <v>1.13</v>
+        <v>1.132</v>
       </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="n">
-        <v>0.923</v>
+        <v>0.926</v>
       </c>
       <c r="O30" t="n">
-        <v>1.13</v>
+        <v>1.132</v>
       </c>
     </row>
     <row r="31">
@@ -1840,34 +1840,34 @@
         <v>7</v>
       </c>
       <c r="D31" t="n">
-        <v>-2.633</v>
+        <v>-2.642</v>
       </c>
       <c r="E31" t="n">
-        <v>-2.379</v>
+        <v>-2.388</v>
       </c>
       <c r="F31" t="n">
-        <v>-2.32</v>
+        <v>-2.329</v>
       </c>
       <c r="G31" t="n">
-        <v>-2.605</v>
+        <v>-2.614</v>
       </c>
       <c r="H31" t="n">
-        <v>-2.64</v>
+        <v>-2.659</v>
       </c>
       <c r="I31" t="n">
-        <v>-2.32</v>
+        <v>-2.329</v>
       </c>
       <c r="J31" t="n">
-        <v>-1.792</v>
+        <v>-1.802</v>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
-        <v>-1.792</v>
+        <v>-1.802</v>
       </c>
       <c r="O31" t="n">
-        <v>-1.792</v>
+        <v>-1.802</v>
       </c>
     </row>
     <row r="32">
@@ -1885,34 +1885,34 @@
         <v>7</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.313</v>
+        <v>-0.318</v>
       </c>
       <c r="E32" t="n">
-        <v>0.021</v>
+        <v>0.017</v>
       </c>
       <c r="F32" t="n">
-        <v>0.001</v>
+        <v>-0.004</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.278</v>
+        <v>-0.283</v>
       </c>
       <c r="H32" t="n">
-        <v>0.548</v>
+        <v>0.552</v>
       </c>
       <c r="I32" t="n">
-        <v>0.548</v>
+        <v>0.552</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.9320000000000001</v>
+        <v>-0.9330000000000001</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="n">
-        <v>-0.9320000000000001</v>
+        <v>-0.9330000000000001</v>
       </c>
       <c r="O32" t="n">
-        <v>0.548</v>
+        <v>0.552</v>
       </c>
     </row>
     <row r="33">
@@ -1930,34 +1930,34 @@
         <v>7</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.473</v>
+        <v>-0.5629999999999999</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.189</v>
+        <v>-0.265</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.158</v>
+        <v>-0.242</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.468</v>
+        <v>-0.529</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.416</v>
+        <v>-0.55</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.158</v>
+        <v>-0.242</v>
       </c>
       <c r="J33" t="n">
-        <v>0.292</v>
+        <v>0.216</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="n">
-        <v>0.292</v>
+        <v>0.216</v>
       </c>
       <c r="O33" t="n">
-        <v>0.292</v>
+        <v>0.216</v>
       </c>
     </row>
     <row r="34">
@@ -1975,34 +1975,34 @@
         <v>7</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.361</v>
+        <v>-0.357</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.082</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.052</v>
+        <v>-0.047</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.336</v>
+        <v>-0.332</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.84</v>
+        <v>-0.832</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.052</v>
+        <v>-0.047</v>
       </c>
       <c r="J34" t="n">
-        <v>0.617</v>
+        <v>0.62</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="n">
-        <v>0.617</v>
+        <v>0.62</v>
       </c>
       <c r="O34" t="n">
-        <v>0.617</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="35">
@@ -2020,34 +2020,34 @@
         <v>7</v>
       </c>
       <c r="D35" t="n">
-        <v>-3.463</v>
+        <v>-3.413</v>
       </c>
       <c r="E35" t="n">
-        <v>-3.209</v>
+        <v>-3.157</v>
       </c>
       <c r="F35" t="n">
-        <v>-3.147</v>
+        <v>-3.096</v>
       </c>
       <c r="G35" t="n">
-        <v>-3.441</v>
+        <v>-3.39</v>
       </c>
       <c r="H35" t="n">
-        <v>-5.263</v>
+        <v>-5.209</v>
       </c>
       <c r="I35" t="n">
-        <v>-3.147</v>
+        <v>-3.096</v>
       </c>
       <c r="J35" t="n">
-        <v>-1.571</v>
+        <v>-1.537</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="n">
-        <v>-1.571</v>
+        <v>-1.537</v>
       </c>
       <c r="O35" t="n">
-        <v>-1.571</v>
+        <v>-1.537</v>
       </c>
     </row>
     <row r="36">
@@ -2065,22 +2065,22 @@
         <v>7</v>
       </c>
       <c r="D36" t="n">
-        <v>-3.092</v>
+        <v>-3.093</v>
       </c>
       <c r="E36" t="n">
-        <v>-2.877</v>
+        <v>-2.878</v>
       </c>
       <c r="F36" t="n">
-        <v>-2.778</v>
+        <v>-2.779</v>
       </c>
       <c r="G36" t="n">
-        <v>-3.076</v>
+        <v>-3.077</v>
       </c>
       <c r="H36" t="n">
-        <v>-3.772</v>
+        <v>-3.752</v>
       </c>
       <c r="I36" t="n">
-        <v>-2.778</v>
+        <v>-2.779</v>
       </c>
       <c r="J36" t="n">
         <v>-1.931</v>
@@ -2110,36 +2110,36 @@
         <v>7</v>
       </c>
       <c r="D37" t="n">
-        <v>0.349</v>
+        <v>0.353</v>
       </c>
       <c r="E37" t="n">
-        <v>0.8159999999999999</v>
+        <v>0.819</v>
       </c>
       <c r="F37" t="n">
-        <v>0.643</v>
+        <v>0.646</v>
       </c>
       <c r="G37" t="n">
-        <v>0.491</v>
+        <v>0.494</v>
       </c>
       <c r="H37" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.615</v>
+        <v>-0.612</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="n">
-        <v>3.321</v>
+        <v>3.326</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="n">
-        <v>3.321</v>
+        <v>3.326</v>
       </c>
       <c r="O37" t="n">
-        <v>3.321</v>
+        <v>3.326</v>
       </c>
     </row>
     <row r="38">
@@ -2157,38 +2157,38 @@
         <v>7</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.023</v>
+        <v>-0.016</v>
       </c>
       <c r="E38" t="n">
+        <v>0.802</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.541</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.392</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.592</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.802</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.758</v>
+      </c>
+      <c r="K38" t="n">
         <v>0.795</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0.533</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.383</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.587</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0.795</v>
-      </c>
-      <c r="J38" t="n">
-        <v>0.753</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0.788</v>
       </c>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="n">
-        <v>0.8139999999999999</v>
+        <v>0.82</v>
       </c>
       <c r="N38" t="n">
-        <v>0.8139999999999999</v>
+        <v>0.82</v>
       </c>
       <c r="O38" t="n">
-        <v>0.8139999999999999</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="39">
@@ -2206,34 +2206,34 @@
         <v>7</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.194</v>
+        <v>-0.191</v>
       </c>
       <c r="E39" t="n">
-        <v>0.149</v>
+        <v>0.152</v>
       </c>
       <c r="F39" t="n">
-        <v>0.122</v>
+        <v>0.125</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.159</v>
+        <v>-0.156</v>
       </c>
       <c r="H39" t="n">
-        <v>0.101</v>
+        <v>0.109</v>
       </c>
       <c r="I39" t="n">
-        <v>0.149</v>
+        <v>0.152</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.7</v>
+        <v>-0.698</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="n">
-        <v>-0.7</v>
+        <v>-0.698</v>
       </c>
       <c r="O39" t="n">
-        <v>0.149</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="40">
@@ -2251,34 +2251,34 @@
         <v>7</v>
       </c>
       <c r="D40" t="n">
-        <v>1.337</v>
+        <v>1.221</v>
       </c>
       <c r="E40" t="n">
-        <v>2.108</v>
+        <v>1.967</v>
       </c>
       <c r="F40" t="n">
-        <v>1.819</v>
+        <v>1.703</v>
       </c>
       <c r="G40" t="n">
-        <v>1.41</v>
+        <v>1.29</v>
       </c>
       <c r="H40" t="n">
-        <v>1.956</v>
+        <v>1.871</v>
       </c>
       <c r="I40" t="n">
-        <v>2.108</v>
+        <v>1.967</v>
       </c>
       <c r="J40" t="n">
-        <v>2.056</v>
+        <v>1.931</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="n">
-        <v>2.056</v>
+        <v>1.931</v>
       </c>
       <c r="O40" t="n">
-        <v>2.108</v>
+        <v>1.967</v>
       </c>
     </row>
     <row r="41">
@@ -2296,36 +2296,36 @@
         <v>7</v>
       </c>
       <c r="D41" t="n">
-        <v>2.979</v>
+        <v>2.999</v>
       </c>
       <c r="E41" t="n">
-        <v>3.291</v>
+        <v>3.311</v>
       </c>
       <c r="F41" t="n">
-        <v>3.273</v>
+        <v>3.292</v>
       </c>
       <c r="G41" t="n">
-        <v>3.009</v>
+        <v>3.029</v>
       </c>
       <c r="H41" t="n">
-        <v>3.313</v>
+        <v>3.338</v>
       </c>
       <c r="I41" t="n">
-        <v>3.313</v>
+        <v>3.338</v>
       </c>
       <c r="J41" t="n">
-        <v>2.762</v>
+        <v>2.777</v>
       </c>
       <c r="K41" t="n">
-        <v>3.309</v>
+        <v>3.342</v>
       </c>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="n">
-        <v>2.762</v>
+        <v>2.777</v>
       </c>
       <c r="O41" t="n">
-        <v>3.309</v>
+        <v>3.342</v>
       </c>
     </row>
     <row r="42">
@@ -2343,34 +2343,34 @@
         <v>7</v>
       </c>
       <c r="D42" t="n">
-        <v>-2.363</v>
+        <v>-2.372</v>
       </c>
       <c r="E42" t="n">
-        <v>-2.109</v>
+        <v>-2.121</v>
       </c>
       <c r="F42" t="n">
-        <v>-2.042</v>
+        <v>-2.052</v>
       </c>
       <c r="G42" t="n">
-        <v>-2.34</v>
+        <v>-2.35</v>
       </c>
       <c r="H42" t="n">
-        <v>-3.333</v>
+        <v>-3.342</v>
       </c>
       <c r="I42" t="n">
-        <v>-2.042</v>
+        <v>-2.052</v>
       </c>
       <c r="J42" t="n">
-        <v>-0.597</v>
+        <v>-0.606</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="n">
-        <v>-0.597</v>
+        <v>-0.606</v>
       </c>
       <c r="O42" t="n">
-        <v>-0.597</v>
+        <v>-0.606</v>
       </c>
     </row>
     <row r="43">
@@ -2388,36 +2388,36 @@
         <v>7</v>
       </c>
       <c r="D43" t="n">
-        <v>2.009</v>
+        <v>2.011</v>
       </c>
       <c r="E43" t="n">
-        <v>2.997</v>
+        <v>2.999</v>
       </c>
       <c r="F43" t="n">
-        <v>2.57</v>
+        <v>2.572</v>
       </c>
       <c r="G43" t="n">
-        <v>2.742</v>
+        <v>2.745</v>
       </c>
       <c r="H43" t="n">
-        <v>2.771</v>
+        <v>2.764</v>
       </c>
       <c r="I43" t="n">
-        <v>2.997</v>
+        <v>2.999</v>
       </c>
       <c r="J43" t="n">
-        <v>3.124</v>
+        <v>3.126</v>
       </c>
       <c r="K43" t="n">
-        <v>3.104</v>
+        <v>3.106</v>
       </c>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="n">
-        <v>3.124</v>
+        <v>3.126</v>
       </c>
       <c r="O43" t="n">
-        <v>3.104</v>
+        <v>3.106</v>
       </c>
     </row>
     <row r="44">
@@ -2447,10 +2447,10 @@
         <v>-1.055</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.694</v>
+        <v>-0.695</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.694</v>
+        <v>-0.695</v>
       </c>
       <c r="J44" t="n">
         <v>-1.159</v>
@@ -2462,7 +2462,7 @@
         <v>-1.159</v>
       </c>
       <c r="O44" t="n">
-        <v>-0.694</v>
+        <v>-0.695</v>
       </c>
     </row>
     <row r="45">
@@ -2480,34 +2480,34 @@
         <v>7</v>
       </c>
       <c r="D45" t="n">
-        <v>-1.09</v>
+        <v>-1.099</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.821</v>
+        <v>-0.83</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.773</v>
+        <v>-0.782</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.064</v>
+        <v>-1.074</v>
       </c>
       <c r="H45" t="n">
-        <v>-1.735</v>
+        <v>-1.739</v>
       </c>
       <c r="I45" t="n">
-        <v>-0.773</v>
+        <v>-0.782</v>
       </c>
       <c r="J45" t="n">
-        <v>-0.155</v>
+        <v>-0.165</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
-        <v>-0.155</v>
+        <v>-0.165</v>
       </c>
       <c r="O45" t="n">
-        <v>-0.155</v>
+        <v>-0.165</v>
       </c>
     </row>
     <row r="46">
@@ -2525,34 +2525,34 @@
         <v>7</v>
       </c>
       <c r="D46" t="n">
-        <v>-3.358</v>
+        <v>-3.361</v>
       </c>
       <c r="E46" t="n">
-        <v>-3.155</v>
+        <v>-3.158</v>
       </c>
       <c r="F46" t="n">
-        <v>-3.037</v>
+        <v>-3.039</v>
       </c>
       <c r="G46" t="n">
-        <v>-3.345</v>
+        <v>-3.348</v>
       </c>
       <c r="H46" t="n">
-        <v>-4.69</v>
+        <v>-4.687</v>
       </c>
       <c r="I46" t="n">
-        <v>-3.037</v>
+        <v>-3.039</v>
       </c>
       <c r="J46" t="n">
-        <v>-0.838</v>
+        <v>-0.84</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="n">
-        <v>-0.838</v>
+        <v>-0.84</v>
       </c>
       <c r="O46" t="n">
-        <v>-0.838</v>
+        <v>-0.84</v>
       </c>
     </row>
     <row r="47">
@@ -2570,36 +2570,36 @@
         <v>7</v>
       </c>
       <c r="D47" t="n">
-        <v>-1.668</v>
+        <v>-1.672</v>
       </c>
       <c r="E47" t="n">
-        <v>-1.391</v>
+        <v>-1.394</v>
       </c>
       <c r="F47" t="n">
-        <v>-1.341</v>
+        <v>-1.345</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.643</v>
+        <v>-1.647</v>
       </c>
       <c r="H47" t="n">
-        <v>-1.367</v>
+        <v>-1.377</v>
       </c>
       <c r="I47" t="n">
-        <v>-1.341</v>
+        <v>-1.345</v>
       </c>
       <c r="J47" t="n">
-        <v>-1</v>
+        <v>-1.005</v>
       </c>
       <c r="K47" t="n">
-        <v>-1.05</v>
+        <v>-1.055</v>
       </c>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="n">
-        <v>-1</v>
+        <v>-1.005</v>
       </c>
       <c r="O47" t="n">
-        <v>-1.05</v>
+        <v>-1.055</v>
       </c>
     </row>
     <row r="48">
@@ -2617,34 +2617,34 @@
         <v>7</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.9370000000000001</v>
+        <v>-0.9340000000000001</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.67</v>
+        <v>-0.668</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.623</v>
+        <v>-0.62</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.916</v>
+        <v>-0.913</v>
       </c>
       <c r="H48" t="n">
-        <v>-1.392</v>
+        <v>-1.384</v>
       </c>
       <c r="I48" t="n">
-        <v>-0.623</v>
+        <v>-0.62</v>
       </c>
       <c r="J48" t="n">
-        <v>-0.392</v>
+        <v>-0.39</v>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="n">
-        <v>-0.392</v>
+        <v>-0.39</v>
       </c>
       <c r="O48" t="n">
-        <v>-0.392</v>
+        <v>-0.39</v>
       </c>
     </row>
     <row r="49">
@@ -2662,38 +2662,38 @@
         <v>7</v>
       </c>
       <c r="D49" t="n">
-        <v>0.351</v>
+        <v>0.359</v>
       </c>
       <c r="E49" t="n">
-        <v>0.675</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="F49" t="n">
-        <v>0.658</v>
+        <v>0.666</v>
       </c>
       <c r="G49" t="n">
-        <v>0.386</v>
+        <v>0.394</v>
       </c>
       <c r="H49" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.544</v>
+      </c>
+      <c r="K49" t="n">
         <v>0.8169999999999999</v>
-      </c>
-      <c r="I49" t="n">
-        <v>0.8169999999999999</v>
-      </c>
-      <c r="J49" t="n">
-        <v>0.533</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0.8129999999999999</v>
       </c>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="n">
-        <v>0.895</v>
+        <v>0.898</v>
       </c>
       <c r="N49" t="n">
-        <v>0.895</v>
+        <v>0.898</v>
       </c>
       <c r="O49" t="n">
-        <v>0.895</v>
+        <v>0.898</v>
       </c>
     </row>
     <row r="50">
@@ -2711,34 +2711,34 @@
         <v>7</v>
       </c>
       <c r="D50" t="n">
-        <v>1.77</v>
+        <v>1.735</v>
       </c>
       <c r="E50" t="n">
-        <v>2.289</v>
+        <v>2.241</v>
       </c>
       <c r="F50" t="n">
-        <v>2.263</v>
+        <v>2.227</v>
       </c>
       <c r="G50" t="n">
-        <v>1.79</v>
+        <v>1.751</v>
       </c>
       <c r="H50" t="n">
-        <v>2.188</v>
+        <v>2.132</v>
       </c>
       <c r="I50" t="n">
-        <v>2.289</v>
+        <v>2.241</v>
       </c>
       <c r="J50" t="n">
-        <v>1.461</v>
+        <v>1.423</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="n">
-        <v>1.461</v>
+        <v>1.423</v>
       </c>
       <c r="O50" t="n">
-        <v>2.289</v>
+        <v>2.241</v>
       </c>
     </row>
     <row r="51">
@@ -2768,10 +2768,10 @@
         <v>0.097</v>
       </c>
       <c r="H51" t="n">
-        <v>0.839</v>
+        <v>0.845</v>
       </c>
       <c r="I51" t="n">
-        <v>0.839</v>
+        <v>0.845</v>
       </c>
       <c r="J51" t="n">
         <v>0.36</v>
@@ -2783,7 +2783,7 @@
         <v>0.36</v>
       </c>
       <c r="O51" t="n">
-        <v>0.839</v>
+        <v>0.845</v>
       </c>
     </row>
     <row r="52">
@@ -2801,34 +2801,34 @@
         <v>7</v>
       </c>
       <c r="D52" t="n">
-        <v>0.83</v>
+        <v>0.834</v>
       </c>
       <c r="E52" t="n">
-        <v>1.116</v>
+        <v>1.121</v>
       </c>
       <c r="F52" t="n">
-        <v>1.144</v>
+        <v>1.149</v>
       </c>
       <c r="G52" t="n">
-        <v>0.855</v>
+        <v>0.86</v>
       </c>
       <c r="H52" t="n">
-        <v>0.906</v>
+        <v>0.911</v>
       </c>
       <c r="I52" t="n">
-        <v>1.144</v>
+        <v>1.149</v>
       </c>
       <c r="J52" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="O52" t="n">
-        <v>1.144</v>
+        <v>1.149</v>
       </c>
     </row>
     <row r="53">
@@ -2846,34 +2846,34 @@
         <v>7</v>
       </c>
       <c r="D53" t="n">
-        <v>0.192</v>
+        <v>0.193</v>
       </c>
       <c r="E53" t="n">
-        <v>0.479</v>
+        <v>0.48</v>
       </c>
       <c r="F53" t="n">
-        <v>0.51</v>
+        <v>0.511</v>
       </c>
       <c r="G53" t="n">
-        <v>0.216</v>
+        <v>0.217</v>
       </c>
       <c r="H53" t="n">
-        <v>0.351</v>
+        <v>0.349</v>
       </c>
       <c r="I53" t="n">
-        <v>0.51</v>
+        <v>0.511</v>
       </c>
       <c r="J53" t="n">
-        <v>0.43</v>
+        <v>0.431</v>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="n">
-        <v>0.43</v>
+        <v>0.431</v>
       </c>
       <c r="O53" t="n">
-        <v>0.51</v>
+        <v>0.511</v>
       </c>
     </row>
     <row r="54">
@@ -2903,7 +2903,7 @@
         <v>2.147</v>
       </c>
       <c r="H54" t="n">
-        <v>1.668</v>
+        <v>1.658</v>
       </c>
       <c r="I54" t="n">
         <v>2.777</v>
@@ -2936,34 +2936,34 @@
         <v>7</v>
       </c>
       <c r="D55" t="n">
-        <v>-2.795</v>
+        <v>-3.318</v>
       </c>
       <c r="E55" t="n">
-        <v>-2.519</v>
+        <v>-3.056</v>
       </c>
       <c r="F55" t="n">
-        <v>-2.477</v>
+        <v>-2.996</v>
       </c>
       <c r="G55" t="n">
-        <v>-2.773</v>
+        <v>-3.309</v>
       </c>
       <c r="H55" t="n">
-        <v>-3.416</v>
+        <v>-4.277</v>
       </c>
       <c r="I55" t="n">
-        <v>-2.477</v>
+        <v>-2.996</v>
       </c>
       <c r="J55" t="n">
-        <v>-1.661</v>
+        <v>-2.258</v>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="n">
-        <v>-1.661</v>
+        <v>-2.258</v>
       </c>
       <c r="O55" t="n">
-        <v>-1.661</v>
+        <v>-2.258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
potential growth interpolation bug fix
</commit_message>
<xml_diff>
--- a/latest_version/output/june_update/results_spb.xlsx
+++ b/latest_version/output/june_update/results_spb.xlsx
@@ -525,34 +525,34 @@
         <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>0.186</v>
+        <v>0.187</v>
       </c>
       <c r="E2" t="n">
-        <v>0.786</v>
+        <v>0.788</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>0.209</v>
+        <v>0.21</v>
       </c>
       <c r="H2" t="n">
-        <v>0.66</v>
+        <v>0.655</v>
       </c>
       <c r="I2" t="n">
-        <v>0.786</v>
+        <v>0.788</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.07099999999999999</v>
+        <v>-0.068</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
-        <v>-0.07099999999999999</v>
+        <v>-0.068</v>
       </c>
       <c r="O2" t="n">
-        <v>0.786</v>
+        <v>0.788</v>
       </c>
     </row>
     <row r="3">
@@ -570,34 +570,34 @@
         <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>0.355</v>
+        <v>0.362</v>
       </c>
       <c r="E3" t="n">
-        <v>1.101</v>
+        <v>1.103</v>
       </c>
       <c r="F3" t="n">
-        <v>0.856</v>
+        <v>0.863</v>
       </c>
       <c r="G3" t="n">
-        <v>0.42</v>
+        <v>0.427</v>
       </c>
       <c r="H3" t="n">
-        <v>0.442</v>
+        <v>0.313</v>
       </c>
       <c r="I3" t="n">
-        <v>1.101</v>
+        <v>1.103</v>
       </c>
       <c r="J3" t="n">
-        <v>0.837</v>
+        <v>0.823</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
-        <v>0.837</v>
+        <v>0.823</v>
       </c>
       <c r="O3" t="n">
-        <v>1.101</v>
+        <v>1.103</v>
       </c>
     </row>
     <row r="4">
@@ -615,34 +615,34 @@
         <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.43</v>
+        <v>-3.455</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.149</v>
+        <v>-3.174</v>
       </c>
       <c r="F4" t="n">
-        <v>-3.036</v>
+        <v>-3.06</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.399</v>
+        <v>-3.424</v>
       </c>
       <c r="H4" t="n">
-        <v>-3.826</v>
+        <v>-3.85</v>
       </c>
       <c r="I4" t="n">
-        <v>-3.036</v>
+        <v>-3.06</v>
       </c>
       <c r="J4" t="n">
-        <v>-2.215</v>
+        <v>-2.225</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
-        <v>-2.215</v>
+        <v>-2.225</v>
       </c>
       <c r="O4" t="n">
-        <v>-2.215</v>
+        <v>-2.225</v>
       </c>
     </row>
     <row r="5">
@@ -660,34 +660,34 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.513</v>
+        <v>-0.592</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.141</v>
+        <v>-0.22</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.105</v>
+        <v>-0.183</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.475</v>
+        <v>-0.554</v>
       </c>
       <c r="H5" t="n">
-        <v>0.302</v>
+        <v>0.209</v>
       </c>
       <c r="I5" t="n">
-        <v>0.302</v>
+        <v>0.209</v>
       </c>
       <c r="J5" t="n">
-        <v>-1.037</v>
+        <v>-1.064</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
-        <v>-1.037</v>
+        <v>-1.064</v>
       </c>
       <c r="O5" t="n">
-        <v>0.302</v>
+        <v>0.209</v>
       </c>
     </row>
     <row r="6">
@@ -705,34 +705,34 @@
         <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2</v>
+        <v>-0.254</v>
       </c>
       <c r="E6" t="n">
-        <v>0.149</v>
+        <v>0.094</v>
       </c>
       <c r="F6" t="n">
-        <v>0.223</v>
+        <v>0.166</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.164</v>
+        <v>-0.218</v>
       </c>
       <c r="H6" t="n">
-        <v>0.003</v>
+        <v>-0.06900000000000001</v>
       </c>
       <c r="I6" t="n">
-        <v>0.223</v>
+        <v>0.166</v>
       </c>
       <c r="J6" t="n">
-        <v>0.583</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
-        <v>0.583</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="O6" t="n">
-        <v>0.583</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -750,34 +750,34 @@
         <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.553</v>
+        <v>-0.542</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.24</v>
+        <v>-0.229</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.153</v>
+        <v>-0.142</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.526</v>
+        <v>-0.515</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.096</v>
+        <v>-1.069</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.153</v>
+        <v>-0.142</v>
       </c>
       <c r="J7" t="n">
-        <v>0.343</v>
+        <v>0.347</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
-        <v>0.343</v>
+        <v>0.347</v>
       </c>
       <c r="O7" t="n">
-        <v>0.343</v>
+        <v>0.347</v>
       </c>
     </row>
     <row r="8">
@@ -795,34 +795,34 @@
         <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.309</v>
+        <v>-3.306</v>
       </c>
       <c r="E8" t="n">
-        <v>-3.025</v>
+        <v>-3.023</v>
       </c>
       <c r="F8" t="n">
-        <v>-2.892</v>
+        <v>-2.89</v>
       </c>
       <c r="G8" t="n">
-        <v>-3.286</v>
+        <v>-3.284</v>
       </c>
       <c r="H8" t="n">
-        <v>-5.677</v>
+        <v>-5.682</v>
       </c>
       <c r="I8" t="n">
-        <v>-2.892</v>
+        <v>-2.89</v>
       </c>
       <c r="J8" t="n">
-        <v>-1.16</v>
+        <v>-1.159</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
-        <v>-1.16</v>
+        <v>-1.159</v>
       </c>
       <c r="O8" t="n">
-        <v>-1.16</v>
+        <v>-1.159</v>
       </c>
     </row>
     <row r="9">
@@ -840,36 +840,36 @@
         <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>-3.33</v>
+        <v>-3.299</v>
       </c>
       <c r="E9" t="n">
-        <v>-3.086</v>
+        <v>-3.055</v>
       </c>
       <c r="F9" t="n">
-        <v>-2.923</v>
+        <v>-2.892</v>
       </c>
       <c r="G9" t="n">
-        <v>-3.308</v>
+        <v>-3.277</v>
       </c>
       <c r="H9" t="n">
-        <v>-4.323</v>
+        <v>-4.271</v>
       </c>
       <c r="I9" t="n">
-        <v>-2.923</v>
+        <v>-2.892</v>
       </c>
       <c r="J9" t="n">
-        <v>-1.885</v>
+        <v>-1.883</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
-        <v>-1.885</v>
+        <v>-1.883</v>
       </c>
       <c r="N9" t="n">
-        <v>-1.885</v>
+        <v>-1.883</v>
       </c>
       <c r="O9" t="n">
-        <v>-1.885</v>
+        <v>-1.883</v>
       </c>
     </row>
     <row r="10">
@@ -887,36 +887,36 @@
         <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>0.842</v>
+        <v>0.861</v>
       </c>
       <c r="E10" t="n">
-        <v>1.338</v>
+        <v>1.357</v>
       </c>
       <c r="F10" t="n">
-        <v>1.126</v>
+        <v>1.171</v>
       </c>
       <c r="G10" t="n">
-        <v>0.992</v>
+        <v>1.011</v>
       </c>
       <c r="H10" t="n">
-        <v>1.38</v>
+        <v>1.434</v>
       </c>
       <c r="I10" t="n">
-        <v>1.38</v>
+        <v>1.434</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.364</v>
+        <v>-0.357</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
-        <v>5.397</v>
+        <v>5.4</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>5.397</v>
+        <v>5.4</v>
       </c>
       <c r="O10" t="n">
-        <v>5.397</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="11">
@@ -934,34 +934,34 @@
         <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0.056</v>
+        <v>-0.057</v>
       </c>
       <c r="E11" t="n">
-        <v>0.786</v>
+        <v>0.789</v>
       </c>
       <c r="F11" t="n">
+        <v>0.407</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H11" t="n">
         <v>0.411</v>
       </c>
-      <c r="G11" t="n">
-        <v>0.608</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.521</v>
-      </c>
       <c r="I11" t="n">
-        <v>0.786</v>
+        <v>0.789</v>
       </c>
       <c r="J11" t="n">
-        <v>0.894</v>
+        <v>0.908</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
-        <v>0.894</v>
+        <v>0.908</v>
       </c>
       <c r="O11" t="n">
-        <v>0.894</v>
+        <v>0.908</v>
       </c>
     </row>
     <row r="12">
@@ -979,34 +979,34 @@
         <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>0.058</v>
+        <v>0.023</v>
       </c>
       <c r="E12" t="n">
-        <v>0.446</v>
+        <v>0.412</v>
       </c>
       <c r="F12" t="n">
-        <v>0.47</v>
+        <v>0.436</v>
       </c>
       <c r="G12" t="n">
-        <v>0.097</v>
+        <v>0.062</v>
       </c>
       <c r="H12" t="n">
-        <v>0.382</v>
+        <v>0.332</v>
       </c>
       <c r="I12" t="n">
-        <v>0.47</v>
+        <v>0.436</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.483</v>
+        <v>-0.491</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
-        <v>-0.483</v>
+        <v>-0.491</v>
       </c>
       <c r="O12" t="n">
-        <v>0.47</v>
+        <v>0.436</v>
       </c>
     </row>
     <row r="13">
@@ -1024,34 +1024,34 @@
         <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>0.953</v>
+        <v>0.955</v>
       </c>
       <c r="E13" t="n">
-        <v>1.725</v>
+        <v>1.715</v>
       </c>
       <c r="F13" t="n">
-        <v>1.445</v>
+        <v>1.448</v>
       </c>
       <c r="G13" t="n">
-        <v>1.037</v>
+        <v>1.038</v>
       </c>
       <c r="H13" t="n">
-        <v>0.898</v>
+        <v>0.627</v>
       </c>
       <c r="I13" t="n">
-        <v>1.725</v>
+        <v>1.715</v>
       </c>
       <c r="J13" t="n">
-        <v>1.613</v>
+        <v>1.57</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
-        <v>1.613</v>
+        <v>1.57</v>
       </c>
       <c r="O13" t="n">
-        <v>1.725</v>
+        <v>1.715</v>
       </c>
     </row>
     <row r="14">
@@ -1072,28 +1072,28 @@
         <v>2.617</v>
       </c>
       <c r="E14" t="n">
-        <v>3.081</v>
+        <v>3.079</v>
       </c>
       <c r="F14" t="n">
         <v>3.094</v>
       </c>
       <c r="G14" t="n">
-        <v>2.642</v>
+        <v>2.641</v>
       </c>
       <c r="H14" t="n">
-        <v>2.854</v>
+        <v>2.838</v>
       </c>
       <c r="I14" t="n">
         <v>3.094</v>
       </c>
       <c r="J14" t="n">
-        <v>2.352</v>
+        <v>2.347</v>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
-        <v>2.352</v>
+        <v>2.347</v>
       </c>
       <c r="O14" t="n">
         <v>3.094</v>
@@ -1114,34 +1114,34 @@
         <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.409</v>
+        <v>-2.457</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.119</v>
+        <v>-2.167</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.991</v>
+        <v>-2.039</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.385</v>
+        <v>-2.433</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.489</v>
+        <v>-3.578</v>
       </c>
       <c r="I15" t="n">
-        <v>-1.991</v>
+        <v>-2.039</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.638</v>
+        <v>-0.647</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>-0.638</v>
+        <v>-0.647</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.638</v>
+        <v>-0.647</v>
       </c>
     </row>
     <row r="16">
@@ -1159,34 +1159,34 @@
         <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>2.228</v>
+        <v>2.2</v>
       </c>
       <c r="E16" t="n">
-        <v>3.296</v>
+        <v>3.27</v>
       </c>
       <c r="F16" t="n">
-        <v>2.715</v>
+        <v>2.687</v>
       </c>
       <c r="G16" t="n">
-        <v>2.547</v>
+        <v>2.458</v>
       </c>
       <c r="H16" t="n">
-        <v>2.502</v>
+        <v>2.246</v>
       </c>
       <c r="I16" t="n">
-        <v>3.296</v>
+        <v>3.27</v>
       </c>
       <c r="J16" t="n">
-        <v>3.182</v>
+        <v>3.131</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
-        <v>3.182</v>
+        <v>3.131</v>
       </c>
       <c r="O16" t="n">
-        <v>3.296</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="17">
@@ -1204,34 +1204,34 @@
         <v>4</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.31</v>
+        <v>-1.283</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.978</v>
+        <v>-0.951</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.909</v>
+        <v>-0.882</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.276</v>
+        <v>-1.25</v>
       </c>
       <c r="H17" t="n">
-        <v>-1.028</v>
+        <v>-0.996</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.909</v>
+        <v>-0.882</v>
       </c>
       <c r="J17" t="n">
-        <v>-1.159</v>
+        <v>-1.15</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
-        <v>-1.159</v>
+        <v>-1.15</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.909</v>
+        <v>-0.882</v>
       </c>
     </row>
     <row r="18">
@@ -1249,34 +1249,34 @@
         <v>4</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.106</v>
+        <v>-1.103</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.8</v>
+        <v>-0.797</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.7</v>
+        <v>-0.698</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.076</v>
+        <v>-1.074</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.946</v>
+        <v>-1.937</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.7</v>
+        <v>-0.698</v>
       </c>
       <c r="J18" t="n">
-        <v>0.021</v>
+        <v>0.018</v>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
-        <v>0.021</v>
+        <v>0.018</v>
       </c>
       <c r="O18" t="n">
-        <v>0.021</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="19">
@@ -1294,34 +1294,34 @@
         <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>-3.405</v>
+        <v>-3.443</v>
       </c>
       <c r="E19" t="n">
-        <v>-3.17</v>
+        <v>-3.208</v>
       </c>
       <c r="F19" t="n">
-        <v>-2.994</v>
+        <v>-3.031</v>
       </c>
       <c r="G19" t="n">
-        <v>-3.387</v>
+        <v>-3.425</v>
       </c>
       <c r="H19" t="n">
-        <v>-5.026</v>
+        <v>-5.081</v>
       </c>
       <c r="I19" t="n">
-        <v>-2.994</v>
+        <v>-3.031</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.734</v>
+        <v>-0.737</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
-        <v>-0.734</v>
+        <v>-0.737</v>
       </c>
       <c r="O19" t="n">
-        <v>-0.734</v>
+        <v>-0.737</v>
       </c>
     </row>
     <row r="20">
@@ -1339,28 +1339,28 @@
         <v>4</v>
       </c>
       <c r="D20" t="n">
-        <v>-2.255</v>
+        <v>-2.289</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.939</v>
+        <v>-1.972</v>
       </c>
       <c r="F20" t="n">
-        <v>-1.836</v>
+        <v>-1.869</v>
       </c>
       <c r="G20" t="n">
-        <v>-2.225</v>
+        <v>-2.259</v>
       </c>
       <c r="H20" t="n">
-        <v>-1.885</v>
+        <v>-1.917</v>
       </c>
       <c r="I20" t="n">
-        <v>-1.836</v>
+        <v>-1.869</v>
       </c>
       <c r="J20" t="n">
-        <v>-1.113</v>
+        <v>-1.111</v>
       </c>
       <c r="K20" t="n">
-        <v>-1.175</v>
+        <v>-1.173</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
@@ -1388,34 +1388,34 @@
         <v>4</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.887</v>
+        <v>-0.927</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.586</v>
+        <v>-0.625</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.469</v>
+        <v>-0.508</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.863</v>
+        <v>-0.903</v>
       </c>
       <c r="H21" t="n">
-        <v>-1.573</v>
+        <v>-1.633</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.469</v>
+        <v>-0.508</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.266</v>
+        <v>-0.272</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
-        <v>-0.266</v>
+        <v>-0.272</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.266</v>
+        <v>-0.272</v>
       </c>
     </row>
     <row r="22">
@@ -1433,34 +1433,34 @@
         <v>4</v>
       </c>
       <c r="D22" t="n">
-        <v>0.003</v>
+        <v>0.034</v>
       </c>
       <c r="E22" t="n">
-        <v>0.375</v>
+        <v>0.405</v>
       </c>
       <c r="F22" t="n">
-        <v>0.412</v>
+        <v>0.442</v>
       </c>
       <c r="G22" t="n">
-        <v>0.045</v>
+        <v>0.075</v>
       </c>
       <c r="H22" t="n">
-        <v>0.698</v>
+        <v>0.717</v>
       </c>
       <c r="I22" t="n">
-        <v>0.698</v>
+        <v>0.717</v>
       </c>
       <c r="J22" t="n">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="O22" t="n">
-        <v>0.698</v>
+        <v>0.717</v>
       </c>
     </row>
     <row r="23">
@@ -1478,34 +1478,34 @@
         <v>4</v>
       </c>
       <c r="D23" t="n">
-        <v>1.966</v>
+        <v>1.967</v>
       </c>
       <c r="E23" t="n">
-        <v>2.504</v>
+        <v>2.495</v>
       </c>
       <c r="F23" t="n">
-        <v>2.462</v>
+        <v>2.463</v>
       </c>
       <c r="G23" t="n">
-        <v>1.981</v>
+        <v>1.982</v>
       </c>
       <c r="H23" t="n">
-        <v>1.952</v>
+        <v>1.737</v>
       </c>
       <c r="I23" t="n">
-        <v>2.504</v>
+        <v>2.495</v>
       </c>
       <c r="J23" t="n">
-        <v>1.627</v>
+        <v>1.591</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="n">
-        <v>1.627</v>
+        <v>1.591</v>
       </c>
       <c r="O23" t="n">
-        <v>2.504</v>
+        <v>2.495</v>
       </c>
     </row>
     <row r="24">
@@ -1523,22 +1523,22 @@
         <v>4</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.627</v>
+        <v>-0.617</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.278</v>
+        <v>-0.267</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.228</v>
+        <v>-0.217</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.591</v>
+        <v>-0.581</v>
       </c>
       <c r="H24" t="n">
-        <v>0.164</v>
+        <v>0.18</v>
       </c>
       <c r="I24" t="n">
-        <v>0.164</v>
+        <v>0.18</v>
       </c>
       <c r="J24" t="n">
         <v>0.406</v>
@@ -1568,34 +1568,34 @@
         <v>4</v>
       </c>
       <c r="D25" t="n">
-        <v>0.504</v>
+        <v>0.514</v>
       </c>
       <c r="E25" t="n">
-        <v>0.829</v>
+        <v>0.839</v>
       </c>
       <c r="F25" t="n">
-        <v>0.908</v>
+        <v>0.918</v>
       </c>
       <c r="G25" t="n">
-        <v>0.535</v>
+        <v>0.545</v>
       </c>
       <c r="H25" t="n">
-        <v>0.729</v>
+        <v>0.752</v>
       </c>
       <c r="I25" t="n">
-        <v>0.908</v>
+        <v>0.918</v>
       </c>
       <c r="J25" t="n">
-        <v>0.443</v>
+        <v>0.448</v>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
-        <v>0.443</v>
+        <v>0.448</v>
       </c>
       <c r="O25" t="n">
-        <v>0.908</v>
+        <v>0.918</v>
       </c>
     </row>
     <row r="26">
@@ -1613,22 +1613,22 @@
         <v>4</v>
       </c>
       <c r="D26" t="n">
-        <v>0.119</v>
+        <v>0.115</v>
       </c>
       <c r="E26" t="n">
-        <v>0.447</v>
+        <v>0.443</v>
       </c>
       <c r="F26" t="n">
-        <v>0.532</v>
+        <v>0.528</v>
       </c>
       <c r="G26" t="n">
-        <v>0.146</v>
+        <v>0.142</v>
       </c>
       <c r="H26" t="n">
-        <v>0.359</v>
+        <v>0.344</v>
       </c>
       <c r="I26" t="n">
-        <v>0.532</v>
+        <v>0.528</v>
       </c>
       <c r="J26" t="n">
         <v>0.368</v>
@@ -1640,7 +1640,7 @@
         <v>0.368</v>
       </c>
       <c r="O26" t="n">
-        <v>0.532</v>
+        <v>0.528</v>
       </c>
     </row>
     <row r="27">
@@ -1658,34 +1658,34 @@
         <v>4</v>
       </c>
       <c r="D27" t="n">
-        <v>2.047</v>
+        <v>2.048</v>
       </c>
       <c r="E27" t="n">
-        <v>2.733</v>
+        <v>2.722</v>
       </c>
       <c r="F27" t="n">
-        <v>2.544</v>
+        <v>2.545</v>
       </c>
       <c r="G27" t="n">
         <v>2.095</v>
       </c>
       <c r="H27" t="n">
-        <v>1.117</v>
+        <v>0.865</v>
       </c>
       <c r="I27" t="n">
-        <v>2.733</v>
+        <v>2.722</v>
       </c>
       <c r="J27" t="n">
-        <v>2.212</v>
+        <v>2.17</v>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="n">
-        <v>2.212</v>
+        <v>2.17</v>
       </c>
       <c r="O27" t="n">
-        <v>2.733</v>
+        <v>2.722</v>
       </c>
     </row>
     <row r="28">
@@ -1703,34 +1703,34 @@
         <v>4</v>
       </c>
       <c r="D28" t="n">
-        <v>-3.311</v>
+        <v>-3.331</v>
       </c>
       <c r="E28" t="n">
-        <v>-3.033</v>
+        <v>-3.052</v>
       </c>
       <c r="F28" t="n">
-        <v>-2.895</v>
+        <v>-2.915</v>
       </c>
       <c r="G28" t="n">
-        <v>-3.304</v>
+        <v>-3.324</v>
       </c>
       <c r="H28" t="n">
-        <v>-4.672</v>
+        <v>-4.704</v>
       </c>
       <c r="I28" t="n">
-        <v>-2.895</v>
+        <v>-2.915</v>
       </c>
       <c r="J28" t="n">
-        <v>-2.089</v>
+        <v>-2.092</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="n">
-        <v>-2.089</v>
+        <v>-2.092</v>
       </c>
       <c r="O28" t="n">
-        <v>-2.089</v>
+        <v>-2.092</v>
       </c>
     </row>
     <row r="29">
@@ -1751,31 +1751,33 @@
         <v>-0.06</v>
       </c>
       <c r="E29" t="n">
-        <v>0.555</v>
+        <v>0.556</v>
       </c>
       <c r="F29" t="n">
         <v>0.447</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.037</v>
+        <v>-0.036</v>
       </c>
       <c r="H29" t="n">
-        <v>0.723</v>
+        <v>0.718</v>
       </c>
       <c r="I29" t="n">
-        <v>0.723</v>
+        <v>0.718</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.227</v>
+        <v>-0.224</v>
       </c>
       <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
+      <c r="L29" t="n">
+        <v>0.732</v>
+      </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="n">
-        <v>-0.227</v>
+        <v>0.732</v>
       </c>
       <c r="O29" t="n">
-        <v>0.723</v>
+        <v>0.732</v>
       </c>
     </row>
     <row r="30">
@@ -1793,25 +1795,25 @@
         <v>7</v>
       </c>
       <c r="D30" t="n">
-        <v>0.391</v>
+        <v>0.397</v>
       </c>
       <c r="E30" t="n">
         <v>1.146</v>
       </c>
       <c r="F30" t="n">
-        <v>0.893</v>
+        <v>0.899</v>
       </c>
       <c r="G30" t="n">
-        <v>0.455</v>
+        <v>0.46</v>
       </c>
       <c r="H30" t="n">
-        <v>0.675</v>
+        <v>0.577</v>
       </c>
       <c r="I30" t="n">
         <v>1.146</v>
       </c>
       <c r="J30" t="n">
-        <v>0.955</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="K30" t="n">
         <v>1.139</v>
@@ -1819,7 +1821,7 @@
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="n">
-        <v>0.955</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="O30" t="n">
         <v>1.139</v>
@@ -1840,34 +1842,34 @@
         <v>7</v>
       </c>
       <c r="D31" t="n">
-        <v>-2.657</v>
+        <v>-2.679</v>
       </c>
       <c r="E31" t="n">
-        <v>-2.401</v>
+        <v>-2.423</v>
       </c>
       <c r="F31" t="n">
-        <v>-2.326</v>
+        <v>-2.347</v>
       </c>
       <c r="G31" t="n">
-        <v>-2.63</v>
+        <v>-2.651</v>
       </c>
       <c r="H31" t="n">
-        <v>-2.68</v>
+        <v>-2.716</v>
       </c>
       <c r="I31" t="n">
-        <v>-2.326</v>
+        <v>-2.347</v>
       </c>
       <c r="J31" t="n">
-        <v>-1.805</v>
+        <v>-1.815</v>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
-        <v>-1.805</v>
+        <v>-1.815</v>
       </c>
       <c r="O31" t="n">
-        <v>-1.805</v>
+        <v>-1.815</v>
       </c>
     </row>
     <row r="32">
@@ -1885,34 +1887,34 @@
         <v>7</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.351</v>
+        <v>-0.423</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.012</v>
+        <v>-0.08400000000000001</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.007</v>
+        <v>-0.078</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.315</v>
+        <v>-0.388</v>
       </c>
       <c r="H32" t="n">
-        <v>0.512</v>
+        <v>0.391</v>
       </c>
       <c r="I32" t="n">
-        <v>0.512</v>
+        <v>0.391</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.961</v>
+        <v>-0.99</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="n">
-        <v>-0.961</v>
+        <v>-0.99</v>
       </c>
       <c r="O32" t="n">
-        <v>0.512</v>
+        <v>0.391</v>
       </c>
     </row>
     <row r="33">
@@ -1930,34 +1932,34 @@
         <v>7</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.666</v>
+        <v>-0.711</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.372</v>
+        <v>-0.416</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.317</v>
+        <v>-0.361</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.655</v>
+        <v>-0.7</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.727</v>
+        <v>-0.8</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.317</v>
+        <v>-0.361</v>
       </c>
       <c r="J33" t="n">
-        <v>0.184</v>
+        <v>0.164</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="n">
-        <v>0.184</v>
+        <v>0.164</v>
       </c>
       <c r="O33" t="n">
-        <v>0.184</v>
+        <v>0.164</v>
       </c>
     </row>
     <row r="34">
@@ -1975,34 +1977,34 @@
         <v>7</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.335</v>
+        <v>-0.325</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.055</v>
+        <v>-0.045</v>
       </c>
       <c r="F34" t="n">
-        <v>0.001</v>
+        <v>0.011</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.309</v>
+        <v>-0.299</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.8129999999999999</v>
+        <v>-0.788</v>
       </c>
       <c r="I34" t="n">
-        <v>0.001</v>
+        <v>0.011</v>
       </c>
       <c r="J34" t="n">
-        <v>0.634</v>
+        <v>0.638</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="n">
-        <v>0.634</v>
+        <v>0.638</v>
       </c>
       <c r="O34" t="n">
-        <v>0.634</v>
+        <v>0.638</v>
       </c>
     </row>
     <row r="35">
@@ -2020,34 +2022,34 @@
         <v>7</v>
       </c>
       <c r="D35" t="n">
-        <v>-3.502</v>
+        <v>-3.501</v>
       </c>
       <c r="E35" t="n">
-        <v>-3.244</v>
+        <v>-3.243</v>
       </c>
       <c r="F35" t="n">
-        <v>-3.147</v>
+        <v>-3.146</v>
       </c>
       <c r="G35" t="n">
-        <v>-3.48</v>
+        <v>-3.478</v>
       </c>
       <c r="H35" t="n">
-        <v>-5.41</v>
+        <v>-5.408</v>
       </c>
       <c r="I35" t="n">
-        <v>-3.147</v>
+        <v>-3.146</v>
       </c>
       <c r="J35" t="n">
-        <v>-1.552</v>
+        <v>-1.551</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="n">
-        <v>-1.552</v>
+        <v>-1.551</v>
       </c>
       <c r="O35" t="n">
-        <v>-1.552</v>
+        <v>-1.551</v>
       </c>
     </row>
     <row r="36">
@@ -2065,34 +2067,34 @@
         <v>7</v>
       </c>
       <c r="D36" t="n">
-        <v>-2.983</v>
+        <v>-2.958</v>
       </c>
       <c r="E36" t="n">
-        <v>-2.763</v>
+        <v>-2.739</v>
       </c>
       <c r="F36" t="n">
-        <v>-2.637</v>
+        <v>-2.613</v>
       </c>
       <c r="G36" t="n">
-        <v>-2.966</v>
+        <v>-2.941</v>
       </c>
       <c r="H36" t="n">
-        <v>-3.588</v>
+        <v>-3.551</v>
       </c>
       <c r="I36" t="n">
-        <v>-2.637</v>
+        <v>-2.613</v>
       </c>
       <c r="J36" t="n">
-        <v>-1.89</v>
+        <v>-1.882</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="n">
-        <v>-1.89</v>
+        <v>-1.882</v>
       </c>
       <c r="O36" t="n">
-        <v>-1.89</v>
+        <v>-1.882</v>
       </c>
     </row>
     <row r="37">
@@ -2110,36 +2112,36 @@
         <v>7</v>
       </c>
       <c r="D37" t="n">
-        <v>0.42</v>
+        <v>0.468</v>
       </c>
       <c r="E37" t="n">
-        <v>0.921</v>
+        <v>0.968</v>
       </c>
       <c r="F37" t="n">
-        <v>0.628</v>
+        <v>0.67</v>
       </c>
       <c r="G37" t="n">
-        <v>0.572</v>
+        <v>0.62</v>
       </c>
       <c r="H37" t="n">
-        <v>0.994</v>
+        <v>1.029</v>
       </c>
       <c r="I37" t="n">
-        <v>0.994</v>
+        <v>1.029</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.59</v>
+        <v>-0.583</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="n">
-        <v>4.012</v>
+        <v>4.045</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="n">
-        <v>4.012</v>
+        <v>4.045</v>
       </c>
       <c r="O37" t="n">
-        <v>4.012</v>
+        <v>4.045</v>
       </c>
     </row>
     <row r="38">
@@ -2157,25 +2159,25 @@
         <v>7</v>
       </c>
       <c r="D38" t="n">
-        <v>0.004</v>
+        <v>-0.02</v>
       </c>
       <c r="E38" t="n">
-        <v>0.8129999999999999</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="F38" t="n">
-        <v>0.48</v>
+        <v>0.474</v>
       </c>
       <c r="G38" t="n">
-        <v>0.621</v>
+        <v>0.505</v>
       </c>
       <c r="H38" t="n">
-        <v>0.591</v>
+        <v>0.548</v>
       </c>
       <c r="I38" t="n">
-        <v>0.8129999999999999</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="J38" t="n">
-        <v>0.987</v>
+        <v>0.988</v>
       </c>
       <c r="K38" t="n">
         <v>0.883</v>
@@ -2183,7 +2185,7 @@
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="n">
-        <v>0.987</v>
+        <v>0.988</v>
       </c>
       <c r="O38" t="n">
         <v>0.883</v>
@@ -2204,34 +2206,34 @@
         <v>7</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.171</v>
+        <v>-0.202</v>
       </c>
       <c r="E39" t="n">
-        <v>0.179</v>
+        <v>0.148</v>
       </c>
       <c r="F39" t="n">
-        <v>0.179</v>
+        <v>0.149</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.136</v>
+        <v>-0.166</v>
       </c>
       <c r="H39" t="n">
-        <v>0.152</v>
+        <v>0.101</v>
       </c>
       <c r="I39" t="n">
-        <v>0.179</v>
+        <v>0.149</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.695</v>
+        <v>-0.703</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="n">
-        <v>-0.695</v>
+        <v>-0.703</v>
       </c>
       <c r="O39" t="n">
-        <v>0.179</v>
+        <v>0.149</v>
       </c>
     </row>
     <row r="40">
@@ -2249,34 +2251,34 @@
         <v>7</v>
       </c>
       <c r="D40" t="n">
-        <v>1.215</v>
+        <v>1.217</v>
       </c>
       <c r="E40" t="n">
-        <v>1.956</v>
+        <v>1.947</v>
       </c>
       <c r="F40" t="n">
-        <v>1.7</v>
+        <v>1.703</v>
       </c>
       <c r="G40" t="n">
         <v>1.28</v>
       </c>
       <c r="H40" t="n">
-        <v>1.893</v>
+        <v>1.662</v>
       </c>
       <c r="I40" t="n">
-        <v>1.956</v>
+        <v>1.947</v>
       </c>
       <c r="J40" t="n">
-        <v>1.907</v>
+        <v>1.864</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="n">
-        <v>1.907</v>
+        <v>1.864</v>
       </c>
       <c r="O40" t="n">
-        <v>1.956</v>
+        <v>1.947</v>
       </c>
     </row>
     <row r="41">
@@ -2294,36 +2296,36 @@
         <v>7</v>
       </c>
       <c r="D41" t="n">
-        <v>3.068</v>
+        <v>3.054</v>
       </c>
       <c r="E41" t="n">
-        <v>3.388</v>
+        <v>3.373</v>
       </c>
       <c r="F41" t="n">
-        <v>3.395</v>
+        <v>3.381</v>
       </c>
       <c r="G41" t="n">
-        <v>3.099</v>
+        <v>3.085</v>
       </c>
       <c r="H41" t="n">
-        <v>3.36</v>
+        <v>3.338</v>
       </c>
       <c r="I41" t="n">
-        <v>3.395</v>
+        <v>3.381</v>
       </c>
       <c r="J41" t="n">
-        <v>2.809</v>
+        <v>2.803</v>
       </c>
       <c r="K41" t="n">
-        <v>3.375</v>
+        <v>3.359</v>
       </c>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="n">
-        <v>2.809</v>
+        <v>2.803</v>
       </c>
       <c r="O41" t="n">
-        <v>3.375</v>
+        <v>3.359</v>
       </c>
     </row>
     <row r="42">
@@ -2341,34 +2343,34 @@
         <v>7</v>
       </c>
       <c r="D42" t="n">
-        <v>-2.421</v>
+        <v>-2.455</v>
       </c>
       <c r="E42" t="n">
-        <v>-2.166</v>
+        <v>-2.2</v>
       </c>
       <c r="F42" t="n">
-        <v>-2.066</v>
+        <v>-2.099</v>
       </c>
       <c r="G42" t="n">
-        <v>-2.398</v>
+        <v>-2.432</v>
       </c>
       <c r="H42" t="n">
-        <v>-3.446</v>
+        <v>-3.519</v>
       </c>
       <c r="I42" t="n">
-        <v>-2.066</v>
+        <v>-2.099</v>
       </c>
       <c r="J42" t="n">
-        <v>-0.612</v>
+        <v>-0.619</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="n">
-        <v>-0.612</v>
+        <v>-0.619</v>
       </c>
       <c r="O42" t="n">
-        <v>-0.612</v>
+        <v>-0.619</v>
       </c>
     </row>
     <row r="43">
@@ -2386,36 +2388,36 @@
         <v>7</v>
       </c>
       <c r="D43" t="n">
-        <v>2.015</v>
+        <v>1.98</v>
       </c>
       <c r="E43" t="n">
-        <v>3.011</v>
+        <v>2.984</v>
       </c>
       <c r="F43" t="n">
-        <v>2.486</v>
+        <v>2.453</v>
       </c>
       <c r="G43" t="n">
-        <v>2.968</v>
+        <v>2.63</v>
       </c>
       <c r="H43" t="n">
-        <v>2.766</v>
+        <v>2.539</v>
       </c>
       <c r="I43" t="n">
-        <v>3.011</v>
+        <v>2.984</v>
       </c>
       <c r="J43" t="n">
-        <v>3.147</v>
+        <v>3.091</v>
       </c>
       <c r="K43" t="n">
-        <v>3.129</v>
+        <v>3.072</v>
       </c>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="n">
-        <v>3.147</v>
+        <v>3.091</v>
       </c>
       <c r="O43" t="n">
-        <v>3.129</v>
+        <v>3.072</v>
       </c>
     </row>
     <row r="44">
@@ -2433,34 +2435,34 @@
         <v>7</v>
       </c>
       <c r="D44" t="n">
-        <v>-1.064</v>
+        <v>-1.04</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.762</v>
+        <v>-0.738</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.725</v>
+        <v>-0.702</v>
       </c>
       <c r="G44" t="n">
-        <v>-1.033</v>
+        <v>-1.009</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.658</v>
+        <v>-0.612</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.658</v>
+        <v>-0.612</v>
       </c>
       <c r="J44" t="n">
-        <v>-1.151</v>
+        <v>-1.142</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="n">
-        <v>-1.151</v>
+        <v>-1.142</v>
       </c>
       <c r="O44" t="n">
-        <v>-0.658</v>
+        <v>-0.612</v>
       </c>
     </row>
     <row r="45">
@@ -2478,34 +2480,34 @@
         <v>7</v>
       </c>
       <c r="D45" t="n">
-        <v>-1.049</v>
+        <v>-1.048</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.775</v>
+        <v>-0.774</v>
       </c>
       <c r="F45" t="n">
         <v>-0.705</v>
       </c>
       <c r="G45" t="n">
-        <v>-1.023</v>
+        <v>-1.022</v>
       </c>
       <c r="H45" t="n">
-        <v>-1.666</v>
+        <v>-1.665</v>
       </c>
       <c r="I45" t="n">
         <v>-0.705</v>
       </c>
       <c r="J45" t="n">
-        <v>-0.146</v>
+        <v>-0.149</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
-        <v>-0.146</v>
+        <v>-0.149</v>
       </c>
       <c r="O45" t="n">
-        <v>-0.146</v>
+        <v>-0.149</v>
       </c>
     </row>
     <row r="46">
@@ -2523,34 +2525,34 @@
         <v>7</v>
       </c>
       <c r="D46" t="n">
-        <v>-3.326</v>
+        <v>-3.353</v>
       </c>
       <c r="E46" t="n">
-        <v>-3.121</v>
+        <v>-3.146</v>
       </c>
       <c r="F46" t="n">
-        <v>-2.975</v>
+        <v>-3.001</v>
       </c>
       <c r="G46" t="n">
-        <v>-3.313</v>
+        <v>-3.34</v>
       </c>
       <c r="H46" t="n">
-        <v>-4.652</v>
+        <v>-4.711</v>
       </c>
       <c r="I46" t="n">
-        <v>-2.975</v>
+        <v>-3.001</v>
       </c>
       <c r="J46" t="n">
-        <v>-0.834</v>
+        <v>-0.835</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="n">
-        <v>-0.834</v>
+        <v>-0.835</v>
       </c>
       <c r="O46" t="n">
-        <v>-0.834</v>
+        <v>-0.835</v>
       </c>
     </row>
     <row r="47">
@@ -2568,36 +2570,36 @@
         <v>7</v>
       </c>
       <c r="D47" t="n">
-        <v>-1.644</v>
+        <v>-1.673</v>
       </c>
       <c r="E47" t="n">
-        <v>-1.362</v>
+        <v>-1.39</v>
       </c>
       <c r="F47" t="n">
-        <v>-1.286</v>
+        <v>-1.313</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.619</v>
+        <v>-1.647</v>
       </c>
       <c r="H47" t="n">
-        <v>-1.317</v>
+        <v>-1.372</v>
       </c>
       <c r="I47" t="n">
-        <v>-1.286</v>
+        <v>-1.313</v>
       </c>
       <c r="J47" t="n">
-        <v>-0.993</v>
+        <v>-1.001</v>
       </c>
       <c r="K47" t="n">
-        <v>-1.058</v>
+        <v>-1.066</v>
       </c>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="n">
-        <v>-0.993</v>
+        <v>-1.001</v>
       </c>
       <c r="O47" t="n">
-        <v>-1.058</v>
+        <v>-1.066</v>
       </c>
     </row>
     <row r="48">
@@ -2615,34 +2617,34 @@
         <v>7</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.888</v>
+        <v>-0.921</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.615</v>
+        <v>-0.648</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.533</v>
+        <v>-0.5659999999999999</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.866</v>
+        <v>-0.9</v>
       </c>
       <c r="H48" t="n">
-        <v>-1.324</v>
+        <v>-1.384</v>
       </c>
       <c r="I48" t="n">
-        <v>-0.533</v>
+        <v>-0.5659999999999999</v>
       </c>
       <c r="J48" t="n">
-        <v>-0.374</v>
+        <v>-0.381</v>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="n">
-        <v>-0.374</v>
+        <v>-0.381</v>
       </c>
       <c r="O48" t="n">
-        <v>-0.374</v>
+        <v>-0.381</v>
       </c>
     </row>
     <row r="49">
@@ -2660,38 +2662,38 @@
         <v>7</v>
       </c>
       <c r="D49" t="n">
-        <v>0.412</v>
+        <v>0.419</v>
       </c>
       <c r="E49" t="n">
-        <v>0.744</v>
+        <v>0.773</v>
       </c>
       <c r="F49" t="n">
-        <v>0.754</v>
+        <v>0.783</v>
       </c>
       <c r="G49" t="n">
-        <v>0.438</v>
+        <v>0.444</v>
       </c>
       <c r="H49" t="n">
-        <v>0.846</v>
+        <v>0.916</v>
       </c>
       <c r="I49" t="n">
-        <v>0.846</v>
+        <v>0.916</v>
       </c>
       <c r="J49" t="n">
-        <v>0.719</v>
+        <v>0.724</v>
       </c>
       <c r="K49" t="n">
-        <v>0.854</v>
+        <v>0.927</v>
       </c>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="n">
-        <v>0.919</v>
+        <v>0.931</v>
       </c>
       <c r="N49" t="n">
-        <v>0.919</v>
+        <v>0.931</v>
       </c>
       <c r="O49" t="n">
-        <v>0.919</v>
+        <v>0.931</v>
       </c>
     </row>
     <row r="50">
@@ -2709,34 +2711,34 @@
         <v>7</v>
       </c>
       <c r="D50" t="n">
-        <v>1.733</v>
+        <v>1.736</v>
       </c>
       <c r="E50" t="n">
-        <v>2.236</v>
+        <v>2.228</v>
       </c>
       <c r="F50" t="n">
-        <v>2.227</v>
+        <v>2.23</v>
       </c>
       <c r="G50" t="n">
-        <v>1.749</v>
+        <v>1.751</v>
       </c>
       <c r="H50" t="n">
-        <v>2.148</v>
+        <v>1.965</v>
       </c>
       <c r="I50" t="n">
-        <v>2.236</v>
+        <v>2.23</v>
       </c>
       <c r="J50" t="n">
-        <v>1.407</v>
+        <v>1.372</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="n">
-        <v>1.407</v>
+        <v>1.372</v>
       </c>
       <c r="O50" t="n">
-        <v>2.236</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="51">
@@ -2754,34 +2756,34 @@
         <v>7</v>
       </c>
       <c r="D51" t="n">
-        <v>0.137</v>
+        <v>0.147</v>
       </c>
       <c r="E51" t="n">
-        <v>0.457</v>
+        <v>0.467</v>
       </c>
       <c r="F51" t="n">
-        <v>0.473</v>
+        <v>0.482</v>
       </c>
       <c r="G51" t="n">
-        <v>0.171</v>
+        <v>0.18</v>
       </c>
       <c r="H51" t="n">
-        <v>0.98</v>
+        <v>0.994</v>
       </c>
       <c r="I51" t="n">
-        <v>0.98</v>
+        <v>0.994</v>
       </c>
       <c r="J51" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="O51" t="n">
-        <v>0.98</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="52">
@@ -2799,34 +2801,34 @@
         <v>7</v>
       </c>
       <c r="D52" t="n">
-        <v>0.897</v>
+        <v>0.907</v>
       </c>
       <c r="E52" t="n">
-        <v>1.189</v>
+        <v>1.199</v>
       </c>
       <c r="F52" t="n">
-        <v>1.237</v>
+        <v>1.247</v>
       </c>
       <c r="G52" t="n">
-        <v>0.923</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="H52" t="n">
-        <v>0.924</v>
+        <v>0.948</v>
       </c>
       <c r="I52" t="n">
-        <v>1.237</v>
+        <v>1.247</v>
       </c>
       <c r="J52" t="n">
-        <v>0.588</v>
+        <v>0.593</v>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="n">
-        <v>0.588</v>
+        <v>0.593</v>
       </c>
       <c r="O52" t="n">
-        <v>1.237</v>
+        <v>1.247</v>
       </c>
     </row>
     <row r="53">
@@ -2844,22 +2846,22 @@
         <v>7</v>
       </c>
       <c r="D53" t="n">
-        <v>0.177</v>
+        <v>0.174</v>
       </c>
       <c r="E53" t="n">
-        <v>0.468</v>
+        <v>0.465</v>
       </c>
       <c r="F53" t="n">
-        <v>0.528</v>
+        <v>0.524</v>
       </c>
       <c r="G53" t="n">
-        <v>0.202</v>
+        <v>0.199</v>
       </c>
       <c r="H53" t="n">
-        <v>0.329</v>
+        <v>0.317</v>
       </c>
       <c r="I53" t="n">
-        <v>0.528</v>
+        <v>0.524</v>
       </c>
       <c r="J53" t="n">
         <v>0.427</v>
@@ -2871,7 +2873,7 @@
         <v>0.427</v>
       </c>
       <c r="O53" t="n">
-        <v>0.528</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="54">
@@ -2892,31 +2894,31 @@
         <v>2.109</v>
       </c>
       <c r="E54" t="n">
-        <v>2.783</v>
+        <v>2.77</v>
       </c>
       <c r="F54" t="n">
         <v>2.602</v>
       </c>
       <c r="G54" t="n">
-        <v>2.149</v>
+        <v>2.147</v>
       </c>
       <c r="H54" t="n">
-        <v>1.674</v>
+        <v>1.428</v>
       </c>
       <c r="I54" t="n">
-        <v>2.783</v>
+        <v>2.77</v>
       </c>
       <c r="J54" t="n">
-        <v>2.283</v>
+        <v>2.24</v>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="n">
-        <v>2.283</v>
+        <v>2.24</v>
       </c>
       <c r="O54" t="n">
-        <v>2.783</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="55">
@@ -2934,34 +2936,34 @@
         <v>7</v>
       </c>
       <c r="D55" t="n">
-        <v>-3.323</v>
+        <v>-3.337</v>
       </c>
       <c r="E55" t="n">
-        <v>-3.056</v>
+        <v>-3.07</v>
       </c>
       <c r="F55" t="n">
-        <v>-2.966</v>
+        <v>-2.98</v>
       </c>
       <c r="G55" t="n">
-        <v>-3.314</v>
+        <v>-3.328</v>
       </c>
       <c r="H55" t="n">
-        <v>-4.317</v>
+        <v>-4.346</v>
       </c>
       <c r="I55" t="n">
-        <v>-2.966</v>
+        <v>-2.98</v>
       </c>
       <c r="J55" t="n">
-        <v>-2.255</v>
+        <v>-2.257</v>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="n">
-        <v>-2.255</v>
+        <v>-2.257</v>
       </c>
       <c r="O55" t="n">
-        <v>-2.255</v>
+        <v>-2.257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>